<commit_message>
up-to-date as of 07/04
</commit_message>
<xml_diff>
--- a/covid_data.xlsx
+++ b/covid_data.xlsx
@@ -529,8 +529,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -544,11 +560,27 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -878,10 +910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK149"/>
+  <dimension ref="A1:AK150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AC1" sqref="AC1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:AD149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -974,8 +1006,12 @@
       <c r="AB1" s="2">
         <v>23</v>
       </c>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
+      <c r="AC1" s="2">
+        <v>29</v>
+      </c>
+      <c r="AD1" s="3">
+        <v>33</v>
+      </c>
       <c r="AE1" s="3"/>
       <c r="AF1" s="3"/>
       <c r="AG1" s="3"/>
@@ -1069,8 +1105,12 @@
       <c r="AB2" s="2">
         <v>111</v>
       </c>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
+      <c r="AC2" s="2">
+        <v>126</v>
+      </c>
+      <c r="AD2" s="3">
+        <v>151</v>
+      </c>
       <c r="AE2" s="3"/>
       <c r="AF2" s="3"/>
       <c r="AG2" s="3"/>
@@ -1164,8 +1204,12 @@
       <c r="AB3" s="2">
         <v>75</v>
       </c>
-      <c r="AC3" s="3"/>
-      <c r="AD3" s="3"/>
+      <c r="AC3" s="2">
+        <v>84</v>
+      </c>
+      <c r="AD3" s="3">
+        <v>100</v>
+      </c>
       <c r="AE3" s="3"/>
       <c r="AF3" s="3"/>
       <c r="AG3" s="3"/>
@@ -1259,8 +1303,12 @@
       <c r="AB4" s="2">
         <v>81</v>
       </c>
-      <c r="AC4" s="3"/>
-      <c r="AD4" s="3"/>
+      <c r="AC4" s="2">
+        <v>108</v>
+      </c>
+      <c r="AD4" s="3">
+        <v>117</v>
+      </c>
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
       <c r="AG4" s="3"/>
@@ -1354,8 +1402,12 @@
       <c r="AB5" s="2">
         <v>32</v>
       </c>
-      <c r="AC5" s="3"/>
-      <c r="AD5" s="3"/>
+      <c r="AC5" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD5" s="3">
+        <v>52</v>
+      </c>
       <c r="AE5" s="3"/>
       <c r="AF5" s="3"/>
       <c r="AG5" s="3"/>
@@ -1449,8 +1501,12 @@
       <c r="AB6" s="2">
         <v>61</v>
       </c>
-      <c r="AC6" s="3"/>
-      <c r="AD6" s="3"/>
+      <c r="AC6" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD6" s="3">
+        <v>95</v>
+      </c>
       <c r="AE6" s="3"/>
       <c r="AF6" s="3"/>
       <c r="AG6" s="3"/>
@@ -1544,8 +1600,12 @@
       <c r="AB7" s="2">
         <v>97</v>
       </c>
-      <c r="AC7" s="3"/>
-      <c r="AD7" s="3"/>
+      <c r="AC7" s="2">
+        <v>122</v>
+      </c>
+      <c r="AD7" s="3">
+        <v>138</v>
+      </c>
       <c r="AE7" s="3"/>
       <c r="AF7" s="3"/>
       <c r="AG7" s="3"/>
@@ -1639,8 +1699,12 @@
       <c r="AB8" s="2">
         <v>52</v>
       </c>
-      <c r="AC8" s="3"/>
-      <c r="AD8" s="3"/>
+      <c r="AC8" s="2">
+        <v>63</v>
+      </c>
+      <c r="AD8" s="3">
+        <v>71</v>
+      </c>
       <c r="AE8" s="3"/>
       <c r="AF8" s="3"/>
       <c r="AG8" s="3"/>
@@ -1734,8 +1798,12 @@
       <c r="AB9" s="2">
         <v>50</v>
       </c>
-      <c r="AC9" s="3"/>
-      <c r="AD9" s="3"/>
+      <c r="AC9" s="2">
+        <v>66</v>
+      </c>
+      <c r="AD9" s="3">
+        <v>72</v>
+      </c>
       <c r="AE9" s="3"/>
       <c r="AF9" s="3"/>
       <c r="AG9" s="3"/>
@@ -1829,8 +1897,12 @@
       <c r="AB10" s="2">
         <v>28</v>
       </c>
-      <c r="AC10" s="3"/>
-      <c r="AD10" s="3"/>
+      <c r="AC10" s="2">
+        <v>31</v>
+      </c>
+      <c r="AD10" s="3">
+        <v>38</v>
+      </c>
       <c r="AE10" s="3"/>
       <c r="AF10" s="3"/>
       <c r="AG10" s="3"/>
@@ -1924,8 +1996,12 @@
       <c r="AB11" s="2">
         <v>78</v>
       </c>
-      <c r="AC11" s="3"/>
-      <c r="AD11" s="3"/>
+      <c r="AC11" s="2">
+        <v>88</v>
+      </c>
+      <c r="AD11" s="3">
+        <v>96</v>
+      </c>
       <c r="AE11" s="3"/>
       <c r="AF11" s="3"/>
       <c r="AG11" s="3"/>
@@ -2019,8 +2095,12 @@
       <c r="AB12" s="2">
         <v>36</v>
       </c>
-      <c r="AC12" s="3"/>
-      <c r="AD12" s="3"/>
+      <c r="AC12" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD12" s="3">
+        <v>49</v>
+      </c>
       <c r="AE12" s="3"/>
       <c r="AF12" s="3"/>
       <c r="AG12" s="3"/>
@@ -2114,8 +2194,12 @@
       <c r="AB13" s="2">
         <v>43</v>
       </c>
-      <c r="AC13" s="3"/>
-      <c r="AD13" s="3"/>
+      <c r="AC13" s="2">
+        <v>51</v>
+      </c>
+      <c r="AD13" s="3">
+        <v>62</v>
+      </c>
       <c r="AE13" s="3"/>
       <c r="AF13" s="3"/>
       <c r="AG13" s="3"/>
@@ -2209,8 +2293,12 @@
       <c r="AB14" s="2">
         <v>57</v>
       </c>
-      <c r="AC14" s="3"/>
-      <c r="AD14" s="3"/>
+      <c r="AC14" s="2">
+        <v>71</v>
+      </c>
+      <c r="AD14" s="3">
+        <v>75</v>
+      </c>
       <c r="AE14" s="3"/>
       <c r="AF14" s="3"/>
       <c r="AG14" s="3"/>
@@ -2304,8 +2392,12 @@
       <c r="AB15" s="2">
         <v>194</v>
       </c>
-      <c r="AC15" s="3"/>
-      <c r="AD15" s="3"/>
+      <c r="AC15" s="2">
+        <v>239</v>
+      </c>
+      <c r="AD15" s="3">
+        <v>263</v>
+      </c>
       <c r="AE15" s="3"/>
       <c r="AF15" s="3"/>
       <c r="AG15" s="3"/>
@@ -2399,8 +2491,12 @@
       <c r="AB16" s="2">
         <v>159</v>
       </c>
-      <c r="AC16" s="3"/>
-      <c r="AD16" s="3"/>
+      <c r="AC16" s="2">
+        <v>195</v>
+      </c>
+      <c r="AD16" s="3">
+        <v>211</v>
+      </c>
       <c r="AE16" s="3"/>
       <c r="AF16" s="3"/>
       <c r="AG16" s="3"/>
@@ -2494,8 +2590,12 @@
       <c r="AB17" s="2">
         <v>6</v>
       </c>
-      <c r="AC17" s="3"/>
-      <c r="AD17" s="3"/>
+      <c r="AC17" s="2">
+        <v>6</v>
+      </c>
+      <c r="AD17" s="3">
+        <v>6</v>
+      </c>
       <c r="AE17" s="3"/>
       <c r="AF17" s="3"/>
       <c r="AG17" s="3"/>
@@ -2589,8 +2689,12 @@
       <c r="AB18" s="2">
         <v>161</v>
       </c>
-      <c r="AC18" s="3"/>
-      <c r="AD18" s="3"/>
+      <c r="AC18" s="2">
+        <v>191</v>
+      </c>
+      <c r="AD18" s="3">
+        <v>204</v>
+      </c>
       <c r="AE18" s="3"/>
       <c r="AF18" s="3"/>
       <c r="AG18" s="3"/>
@@ -2684,8 +2788,12 @@
       <c r="AB19" s="2">
         <v>57</v>
       </c>
-      <c r="AC19" s="3"/>
-      <c r="AD19" s="3"/>
+      <c r="AC19" s="2">
+        <v>62</v>
+      </c>
+      <c r="AD19" s="3">
+        <v>66</v>
+      </c>
       <c r="AE19" s="3"/>
       <c r="AF19" s="3"/>
       <c r="AG19" s="3"/>
@@ -2779,8 +2887,12 @@
       <c r="AB20" s="2">
         <v>70</v>
       </c>
-      <c r="AC20" s="3"/>
-      <c r="AD20" s="3"/>
+      <c r="AC20" s="2">
+        <v>73</v>
+      </c>
+      <c r="AD20" s="3">
+        <v>73</v>
+      </c>
       <c r="AE20" s="3"/>
       <c r="AF20" s="3"/>
       <c r="AG20" s="3"/>
@@ -2874,8 +2986,12 @@
       <c r="AB21" s="2">
         <v>80</v>
       </c>
-      <c r="AC21" s="3"/>
-      <c r="AD21" s="3"/>
+      <c r="AC21" s="2">
+        <v>106</v>
+      </c>
+      <c r="AD21" s="3">
+        <v>115</v>
+      </c>
       <c r="AE21" s="3"/>
       <c r="AF21" s="3"/>
       <c r="AG21" s="3"/>
@@ -2969,8 +3085,12 @@
       <c r="AB22" s="2">
         <v>58</v>
       </c>
-      <c r="AC22" s="3"/>
-      <c r="AD22" s="3"/>
+      <c r="AC22" s="2">
+        <v>58</v>
+      </c>
+      <c r="AD22" s="3">
+        <v>66</v>
+      </c>
       <c r="AE22" s="3"/>
       <c r="AF22" s="3"/>
       <c r="AG22" s="3"/>
@@ -3064,8 +3184,12 @@
       <c r="AB23" s="2">
         <v>166</v>
       </c>
-      <c r="AC23" s="3"/>
-      <c r="AD23" s="3"/>
+      <c r="AC23" s="2">
+        <v>167</v>
+      </c>
+      <c r="AD23" s="3">
+        <v>211</v>
+      </c>
       <c r="AE23" s="3"/>
       <c r="AF23" s="3"/>
       <c r="AG23" s="3"/>
@@ -3159,8 +3283,12 @@
       <c r="AB24" s="2">
         <v>66</v>
       </c>
-      <c r="AC24" s="3"/>
-      <c r="AD24" s="3"/>
+      <c r="AC24" s="2">
+        <v>66</v>
+      </c>
+      <c r="AD24" s="3">
+        <v>82</v>
+      </c>
       <c r="AE24" s="3"/>
       <c r="AF24" s="3"/>
       <c r="AG24" s="3"/>
@@ -3254,8 +3382,12 @@
       <c r="AB25" s="2">
         <v>113</v>
       </c>
-      <c r="AC25" s="3"/>
-      <c r="AD25" s="3"/>
+      <c r="AC25" s="2">
+        <v>113</v>
+      </c>
+      <c r="AD25" s="3">
+        <v>139</v>
+      </c>
       <c r="AE25" s="3"/>
       <c r="AF25" s="3"/>
       <c r="AG25" s="3"/>
@@ -3349,8 +3481,12 @@
       <c r="AB26" s="2">
         <v>71</v>
       </c>
-      <c r="AC26" s="3"/>
-      <c r="AD26" s="3"/>
+      <c r="AC26" s="2">
+        <v>97</v>
+      </c>
+      <c r="AD26" s="3">
+        <v>102</v>
+      </c>
       <c r="AE26" s="3"/>
       <c r="AF26" s="3"/>
       <c r="AG26" s="3"/>
@@ -3444,8 +3580,12 @@
       <c r="AB27" s="2">
         <v>53</v>
       </c>
-      <c r="AC27" s="3"/>
-      <c r="AD27" s="3"/>
+      <c r="AC27" s="2">
+        <v>54</v>
+      </c>
+      <c r="AD27" s="3">
+        <v>57</v>
+      </c>
       <c r="AE27" s="3"/>
       <c r="AF27" s="3"/>
       <c r="AG27" s="3"/>
@@ -3539,8 +3679,12 @@
       <c r="AB28" s="2">
         <v>49</v>
       </c>
-      <c r="AC28" s="3"/>
-      <c r="AD28" s="3"/>
+      <c r="AC28" s="2">
+        <v>50</v>
+      </c>
+      <c r="AD28" s="3">
+        <v>74</v>
+      </c>
       <c r="AE28" s="3"/>
       <c r="AF28" s="3"/>
       <c r="AG28" s="3"/>
@@ -3634,8 +3778,12 @@
       <c r="AB29" s="2">
         <v>48</v>
       </c>
-      <c r="AC29" s="3"/>
-      <c r="AD29" s="3"/>
+      <c r="AC29" s="2">
+        <v>48</v>
+      </c>
+      <c r="AD29" s="3">
+        <v>61</v>
+      </c>
       <c r="AE29" s="3"/>
       <c r="AF29" s="3"/>
       <c r="AG29" s="3"/>
@@ -3729,8 +3877,12 @@
       <c r="AB30" s="2">
         <v>128</v>
       </c>
-      <c r="AC30" s="3"/>
-      <c r="AD30" s="3"/>
+      <c r="AC30" s="2">
+        <v>163</v>
+      </c>
+      <c r="AD30" s="3">
+        <v>167</v>
+      </c>
       <c r="AE30" s="3"/>
       <c r="AF30" s="3"/>
       <c r="AG30" s="3"/>
@@ -3824,8 +3976,12 @@
       <c r="AB31" s="2">
         <v>76</v>
       </c>
-      <c r="AC31" s="3"/>
-      <c r="AD31" s="3"/>
+      <c r="AC31" s="2">
+        <v>97</v>
+      </c>
+      <c r="AD31" s="3">
+        <v>118</v>
+      </c>
       <c r="AE31" s="3"/>
       <c r="AF31" s="3"/>
       <c r="AG31" s="3"/>
@@ -3919,8 +4075,12 @@
       <c r="AB32" s="2">
         <v>83</v>
       </c>
-      <c r="AC32" s="3"/>
-      <c r="AD32" s="3"/>
+      <c r="AC32" s="2">
+        <v>105</v>
+      </c>
+      <c r="AD32" s="3">
+        <v>120</v>
+      </c>
       <c r="AE32" s="3"/>
       <c r="AF32" s="3"/>
       <c r="AG32" s="3"/>
@@ -4014,8 +4174,12 @@
       <c r="AB33" s="2">
         <v>144</v>
       </c>
-      <c r="AC33" s="3"/>
-      <c r="AD33" s="3"/>
+      <c r="AC33" s="2">
+        <v>153</v>
+      </c>
+      <c r="AD33" s="3">
+        <v>153</v>
+      </c>
       <c r="AE33" s="3"/>
       <c r="AF33" s="3"/>
       <c r="AG33" s="3"/>
@@ -4109,8 +4273,12 @@
       <c r="AB34" s="2">
         <v>45</v>
       </c>
-      <c r="AC34" s="3"/>
-      <c r="AD34" s="3"/>
+      <c r="AC34" s="2">
+        <v>57</v>
+      </c>
+      <c r="AD34" s="3">
+        <v>69</v>
+      </c>
       <c r="AE34" s="3"/>
       <c r="AF34" s="3"/>
       <c r="AG34" s="3"/>
@@ -4204,8 +4372,12 @@
       <c r="AB35" s="2">
         <v>74</v>
       </c>
-      <c r="AC35" s="3"/>
-      <c r="AD35" s="3"/>
+      <c r="AC35" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD35" s="3">
+        <v>92</v>
+      </c>
       <c r="AE35" s="3"/>
       <c r="AF35" s="3"/>
       <c r="AG35" s="3"/>
@@ -4299,8 +4471,12 @@
       <c r="AB36" s="2">
         <v>79</v>
       </c>
-      <c r="AC36" s="3"/>
-      <c r="AD36" s="3"/>
+      <c r="AC36" s="2">
+        <v>89</v>
+      </c>
+      <c r="AD36" s="3">
+        <v>111</v>
+      </c>
       <c r="AE36" s="3"/>
       <c r="AF36" s="3"/>
       <c r="AG36" s="3"/>
@@ -4394,8 +4570,12 @@
       <c r="AB37" s="2">
         <v>129</v>
       </c>
-      <c r="AC37" s="3"/>
-      <c r="AD37" s="3"/>
+      <c r="AC37" s="2">
+        <v>143</v>
+      </c>
+      <c r="AD37" s="3">
+        <v>155</v>
+      </c>
       <c r="AE37" s="3"/>
       <c r="AF37" s="3"/>
       <c r="AG37" s="3"/>
@@ -4489,8 +4669,12 @@
       <c r="AB38" s="2">
         <v>88</v>
       </c>
-      <c r="AC38" s="3"/>
-      <c r="AD38" s="3"/>
+      <c r="AC38" s="2">
+        <v>99</v>
+      </c>
+      <c r="AD38" s="3">
+        <v>105</v>
+      </c>
       <c r="AE38" s="3"/>
       <c r="AF38" s="3"/>
       <c r="AG38" s="3"/>
@@ -4584,8 +4768,12 @@
       <c r="AB39" s="2">
         <v>83</v>
       </c>
-      <c r="AC39" s="3"/>
-      <c r="AD39" s="3"/>
+      <c r="AC39" s="2">
+        <v>101</v>
+      </c>
+      <c r="AD39" s="3">
+        <v>114</v>
+      </c>
       <c r="AE39" s="3"/>
       <c r="AF39" s="3"/>
       <c r="AG39" s="3"/>
@@ -4679,8 +4867,12 @@
       <c r="AB40" s="2">
         <v>149</v>
       </c>
-      <c r="AC40" s="3"/>
-      <c r="AD40" s="3"/>
+      <c r="AC40" s="2">
+        <v>155</v>
+      </c>
+      <c r="AD40" s="3">
+        <v>181</v>
+      </c>
       <c r="AE40" s="3"/>
       <c r="AF40" s="3"/>
       <c r="AG40" s="3"/>
@@ -4774,8 +4966,12 @@
       <c r="AB41" s="2">
         <v>73</v>
       </c>
-      <c r="AC41" s="3"/>
-      <c r="AD41" s="3"/>
+      <c r="AC41" s="2">
+        <v>84</v>
+      </c>
+      <c r="AD41" s="3">
+        <v>85</v>
+      </c>
       <c r="AE41" s="3"/>
       <c r="AF41" s="3"/>
       <c r="AG41" s="3"/>
@@ -4869,8 +5065,12 @@
       <c r="AB42" s="2">
         <v>89</v>
       </c>
-      <c r="AC42" s="3"/>
-      <c r="AD42" s="3"/>
+      <c r="AC42" s="2">
+        <v>96</v>
+      </c>
+      <c r="AD42" s="3">
+        <v>104</v>
+      </c>
       <c r="AE42" s="3"/>
       <c r="AF42" s="3"/>
       <c r="AG42" s="3"/>
@@ -4964,8 +5164,12 @@
       <c r="AB43" s="2">
         <v>145</v>
       </c>
-      <c r="AC43" s="3"/>
-      <c r="AD43" s="3"/>
+      <c r="AC43" s="2">
+        <v>147</v>
+      </c>
+      <c r="AD43" s="3">
+        <v>149</v>
+      </c>
       <c r="AE43" s="3"/>
       <c r="AF43" s="3"/>
       <c r="AG43" s="3"/>
@@ -5059,8 +5263,12 @@
       <c r="AB44" s="2">
         <v>25</v>
       </c>
-      <c r="AC44" s="3"/>
-      <c r="AD44" s="3"/>
+      <c r="AC44" s="2">
+        <v>32</v>
+      </c>
+      <c r="AD44" s="3">
+        <v>32</v>
+      </c>
       <c r="AE44" s="3"/>
       <c r="AF44" s="3"/>
       <c r="AG44" s="3"/>
@@ -5154,8 +5362,12 @@
       <c r="AB45" s="2">
         <v>199</v>
       </c>
-      <c r="AC45" s="3"/>
-      <c r="AD45" s="3"/>
+      <c r="AC45" s="2">
+        <v>260</v>
+      </c>
+      <c r="AD45" s="3">
+        <v>292</v>
+      </c>
       <c r="AE45" s="3"/>
       <c r="AF45" s="3"/>
       <c r="AG45" s="3"/>
@@ -5249,8 +5461,12 @@
       <c r="AB46" s="2">
         <v>144</v>
       </c>
-      <c r="AC46" s="3"/>
-      <c r="AD46" s="3"/>
+      <c r="AC46" s="2">
+        <v>171</v>
+      </c>
+      <c r="AD46" s="3">
+        <v>196</v>
+      </c>
       <c r="AE46" s="3"/>
       <c r="AF46" s="3"/>
       <c r="AG46" s="3"/>
@@ -5344,8 +5560,12 @@
       <c r="AB47" s="2">
         <v>149</v>
       </c>
-      <c r="AC47" s="3"/>
-      <c r="AD47" s="3"/>
+      <c r="AC47" s="2">
+        <v>167</v>
+      </c>
+      <c r="AD47" s="3">
+        <v>200</v>
+      </c>
       <c r="AE47" s="3"/>
       <c r="AF47" s="3"/>
       <c r="AG47" s="3"/>
@@ -5439,8 +5659,12 @@
       <c r="AB48" s="2">
         <v>138</v>
       </c>
-      <c r="AC48" s="3"/>
-      <c r="AD48" s="3"/>
+      <c r="AC48" s="2">
+        <v>143</v>
+      </c>
+      <c r="AD48" s="3">
+        <v>143</v>
+      </c>
       <c r="AE48" s="3"/>
       <c r="AF48" s="3"/>
       <c r="AG48" s="3"/>
@@ -5534,8 +5758,12 @@
       <c r="AB49" s="2">
         <v>149</v>
       </c>
-      <c r="AC49" s="3"/>
-      <c r="AD49" s="3"/>
+      <c r="AC49" s="2">
+        <v>187</v>
+      </c>
+      <c r="AD49" s="3">
+        <v>198</v>
+      </c>
       <c r="AE49" s="3"/>
       <c r="AF49" s="3"/>
       <c r="AG49" s="3"/>
@@ -5629,8 +5857,12 @@
       <c r="AB50" s="2">
         <v>120</v>
       </c>
-      <c r="AC50" s="3"/>
-      <c r="AD50" s="3"/>
+      <c r="AC50" s="2">
+        <v>120</v>
+      </c>
+      <c r="AD50" s="3">
+        <v>154</v>
+      </c>
       <c r="AE50" s="3"/>
       <c r="AF50" s="3"/>
       <c r="AG50" s="3"/>
@@ -5724,8 +5956,12 @@
       <c r="AB51" s="2">
         <v>83</v>
       </c>
-      <c r="AC51" s="3"/>
-      <c r="AD51" s="3"/>
+      <c r="AC51" s="2">
+        <v>97</v>
+      </c>
+      <c r="AD51" s="3">
+        <v>110</v>
+      </c>
       <c r="AE51" s="3"/>
       <c r="AF51" s="3"/>
       <c r="AG51" s="3"/>
@@ -5819,8 +6055,12 @@
       <c r="AB52" s="2">
         <v>116</v>
       </c>
-      <c r="AC52" s="3"/>
-      <c r="AD52" s="3"/>
+      <c r="AC52" s="2">
+        <v>132</v>
+      </c>
+      <c r="AD52" s="3">
+        <v>144</v>
+      </c>
       <c r="AE52" s="3"/>
       <c r="AF52" s="3"/>
       <c r="AG52" s="3"/>
@@ -5914,8 +6154,12 @@
       <c r="AB53" s="2">
         <v>142</v>
       </c>
-      <c r="AC53" s="3"/>
-      <c r="AD53" s="3"/>
+      <c r="AC53" s="2">
+        <v>188</v>
+      </c>
+      <c r="AD53" s="3">
+        <v>211</v>
+      </c>
       <c r="AE53" s="3"/>
       <c r="AF53" s="3"/>
       <c r="AG53" s="3"/>
@@ -6009,8 +6253,12 @@
       <c r="AB54" s="2">
         <v>83</v>
       </c>
-      <c r="AC54" s="3"/>
-      <c r="AD54" s="3"/>
+      <c r="AC54" s="2">
+        <v>85</v>
+      </c>
+      <c r="AD54" s="3">
+        <v>115</v>
+      </c>
       <c r="AE54" s="3"/>
       <c r="AF54" s="3"/>
       <c r="AG54" s="3"/>
@@ -6104,8 +6352,12 @@
       <c r="AB55" s="2">
         <v>91</v>
       </c>
-      <c r="AC55" s="3"/>
-      <c r="AD55" s="3"/>
+      <c r="AC55" s="2">
+        <v>95</v>
+      </c>
+      <c r="AD55" s="3">
+        <v>126</v>
+      </c>
       <c r="AE55" s="3"/>
       <c r="AF55" s="3"/>
       <c r="AG55" s="3"/>
@@ -6199,8 +6451,12 @@
       <c r="AB56" s="2">
         <v>109</v>
       </c>
-      <c r="AC56" s="3"/>
-      <c r="AD56" s="3"/>
+      <c r="AC56" s="2">
+        <v>133</v>
+      </c>
+      <c r="AD56" s="3">
+        <v>170</v>
+      </c>
       <c r="AE56" s="3"/>
       <c r="AF56" s="3"/>
       <c r="AG56" s="3"/>
@@ -6294,8 +6550,12 @@
       <c r="AB57" s="2">
         <v>104</v>
       </c>
-      <c r="AC57" s="3"/>
-      <c r="AD57" s="3"/>
+      <c r="AC57" s="2">
+        <v>124</v>
+      </c>
+      <c r="AD57" s="3">
+        <v>138</v>
+      </c>
       <c r="AE57" s="3"/>
       <c r="AF57" s="3"/>
       <c r="AG57" s="3"/>
@@ -6389,8 +6649,12 @@
       <c r="AB58" s="2">
         <v>252</v>
       </c>
-      <c r="AC58" s="3"/>
-      <c r="AD58" s="3"/>
+      <c r="AC58" s="2">
+        <v>293</v>
+      </c>
+      <c r="AD58" s="3">
+        <v>323</v>
+      </c>
       <c r="AE58" s="3"/>
       <c r="AF58" s="3"/>
       <c r="AG58" s="3"/>
@@ -6484,8 +6748,12 @@
       <c r="AB59" s="2">
         <v>152</v>
       </c>
-      <c r="AC59" s="3"/>
-      <c r="AD59" s="3"/>
+      <c r="AC59" s="2">
+        <v>194</v>
+      </c>
+      <c r="AD59" s="3">
+        <v>216</v>
+      </c>
       <c r="AE59" s="3"/>
       <c r="AF59" s="3"/>
       <c r="AG59" s="3"/>
@@ -6579,8 +6847,12 @@
       <c r="AB60" s="2">
         <v>127</v>
       </c>
-      <c r="AC60" s="3"/>
-      <c r="AD60" s="3"/>
+      <c r="AC60" s="2">
+        <v>155</v>
+      </c>
+      <c r="AD60" s="3">
+        <v>167</v>
+      </c>
       <c r="AE60" s="3"/>
       <c r="AF60" s="3"/>
       <c r="AG60" s="3"/>
@@ -6674,8 +6946,12 @@
       <c r="AB61" s="2">
         <v>191</v>
       </c>
-      <c r="AC61" s="3"/>
-      <c r="AD61" s="3"/>
+      <c r="AC61" s="2">
+        <v>226</v>
+      </c>
+      <c r="AD61" s="3">
+        <v>242</v>
+      </c>
       <c r="AE61" s="3"/>
       <c r="AF61" s="3"/>
       <c r="AG61" s="3"/>
@@ -6769,8 +7045,12 @@
       <c r="AB62" s="2">
         <v>193</v>
       </c>
-      <c r="AC62" s="3"/>
-      <c r="AD62" s="3"/>
+      <c r="AC62" s="2">
+        <v>225</v>
+      </c>
+      <c r="AD62" s="3">
+        <v>246</v>
+      </c>
       <c r="AE62" s="3"/>
       <c r="AF62" s="3"/>
       <c r="AG62" s="3"/>
@@ -6864,8 +7144,12 @@
       <c r="AB63" s="2">
         <v>129</v>
       </c>
-      <c r="AC63" s="3"/>
-      <c r="AD63" s="3"/>
+      <c r="AC63" s="2">
+        <v>145</v>
+      </c>
+      <c r="AD63" s="3">
+        <v>162</v>
+      </c>
       <c r="AE63" s="3"/>
       <c r="AF63" s="3"/>
       <c r="AG63" s="3"/>
@@ -6959,8 +7243,12 @@
       <c r="AB64" s="2">
         <v>173</v>
       </c>
-      <c r="AC64" s="3"/>
-      <c r="AD64" s="3"/>
+      <c r="AC64" s="2">
+        <v>201</v>
+      </c>
+      <c r="AD64" s="3">
+        <v>222</v>
+      </c>
       <c r="AE64" s="3"/>
       <c r="AF64" s="3"/>
       <c r="AG64" s="3"/>
@@ -7054,8 +7342,12 @@
       <c r="AB65" s="2">
         <v>116</v>
       </c>
-      <c r="AC65" s="3"/>
-      <c r="AD65" s="3"/>
+      <c r="AC65" s="2">
+        <v>156</v>
+      </c>
+      <c r="AD65" s="3">
+        <v>185</v>
+      </c>
       <c r="AE65" s="3"/>
       <c r="AF65" s="3"/>
       <c r="AG65" s="3"/>
@@ -7149,8 +7441,12 @@
       <c r="AB66" s="2">
         <v>110</v>
       </c>
-      <c r="AC66" s="3"/>
-      <c r="AD66" s="3"/>
+      <c r="AC66" s="2">
+        <v>133</v>
+      </c>
+      <c r="AD66" s="3">
+        <v>167</v>
+      </c>
       <c r="AE66" s="3"/>
       <c r="AF66" s="3"/>
       <c r="AG66" s="3"/>
@@ -7244,8 +7540,12 @@
       <c r="AB67" s="2">
         <v>387</v>
       </c>
-      <c r="AC67" s="3"/>
-      <c r="AD67" s="3"/>
+      <c r="AC67" s="2">
+        <v>455</v>
+      </c>
+      <c r="AD67" s="3">
+        <v>510</v>
+      </c>
       <c r="AE67" s="3"/>
       <c r="AF67" s="3"/>
       <c r="AG67" s="3"/>
@@ -7339,8 +7639,12 @@
       <c r="AB68" s="2">
         <v>148</v>
       </c>
-      <c r="AC68" s="3"/>
-      <c r="AD68" s="3"/>
+      <c r="AC68" s="2">
+        <v>184</v>
+      </c>
+      <c r="AD68" s="3">
+        <v>236</v>
+      </c>
       <c r="AE68" s="3"/>
       <c r="AF68" s="3"/>
       <c r="AG68" s="3"/>
@@ -7434,8 +7738,12 @@
       <c r="AB69" s="2">
         <v>172</v>
       </c>
-      <c r="AC69" s="3"/>
-      <c r="AD69" s="3"/>
+      <c r="AC69" s="2">
+        <v>219</v>
+      </c>
+      <c r="AD69" s="3">
+        <v>264</v>
+      </c>
       <c r="AE69" s="3"/>
       <c r="AF69" s="3"/>
       <c r="AG69" s="3"/>
@@ -7529,8 +7837,12 @@
       <c r="AB70" s="2">
         <v>147</v>
       </c>
-      <c r="AC70" s="3"/>
-      <c r="AD70" s="3"/>
+      <c r="AC70" s="2">
+        <v>168</v>
+      </c>
+      <c r="AD70" s="3">
+        <v>220</v>
+      </c>
       <c r="AE70" s="3"/>
       <c r="AF70" s="3"/>
       <c r="AG70" s="3"/>
@@ -7624,8 +7936,12 @@
       <c r="AB71" s="2">
         <v>158</v>
       </c>
-      <c r="AC71" s="3"/>
-      <c r="AD71" s="3"/>
+      <c r="AC71" s="2">
+        <v>200</v>
+      </c>
+      <c r="AD71" s="3">
+        <v>216</v>
+      </c>
       <c r="AE71" s="3"/>
       <c r="AF71" s="3"/>
       <c r="AG71" s="3"/>
@@ -7719,8 +8035,12 @@
       <c r="AB72" s="2">
         <v>117</v>
       </c>
-      <c r="AC72" s="3"/>
-      <c r="AD72" s="3"/>
+      <c r="AC72" s="2">
+        <v>137</v>
+      </c>
+      <c r="AD72" s="3">
+        <v>144</v>
+      </c>
       <c r="AE72" s="3"/>
       <c r="AF72" s="3"/>
       <c r="AG72" s="3"/>
@@ -7814,8 +8134,12 @@
       <c r="AB73" s="2">
         <v>158</v>
       </c>
-      <c r="AC73" s="3"/>
-      <c r="AD73" s="3"/>
+      <c r="AC73" s="2">
+        <v>202</v>
+      </c>
+      <c r="AD73" s="3">
+        <v>221</v>
+      </c>
       <c r="AE73" s="3"/>
       <c r="AF73" s="3"/>
       <c r="AG73" s="3"/>
@@ -7909,8 +8233,12 @@
       <c r="AB74" s="2">
         <v>730</v>
       </c>
-      <c r="AC74" s="3"/>
-      <c r="AD74" s="3"/>
+      <c r="AC74" s="2">
+        <v>833</v>
+      </c>
+      <c r="AD74" s="3">
+        <v>882</v>
+      </c>
       <c r="AE74" s="3"/>
       <c r="AF74" s="3"/>
       <c r="AG74" s="3"/>
@@ -8004,8 +8332,12 @@
       <c r="AB75" s="2">
         <v>285</v>
       </c>
-      <c r="AC75" s="3"/>
-      <c r="AD75" s="3"/>
+      <c r="AC75" s="2">
+        <v>348</v>
+      </c>
+      <c r="AD75" s="3">
+        <v>359</v>
+      </c>
       <c r="AE75" s="3"/>
       <c r="AF75" s="3"/>
       <c r="AG75" s="3"/>
@@ -8099,8 +8431,12 @@
       <c r="AB76" s="2">
         <v>133</v>
       </c>
-      <c r="AC76" s="3"/>
-      <c r="AD76" s="3"/>
+      <c r="AC76" s="2">
+        <v>160</v>
+      </c>
+      <c r="AD76" s="3">
+        <v>180</v>
+      </c>
       <c r="AE76" s="3"/>
       <c r="AF76" s="3"/>
       <c r="AG76" s="3"/>
@@ -8194,8 +8530,12 @@
       <c r="AB77" s="2">
         <v>57</v>
       </c>
-      <c r="AC77" s="3"/>
-      <c r="AD77" s="3"/>
+      <c r="AC77" s="2">
+        <v>84</v>
+      </c>
+      <c r="AD77" s="3">
+        <v>98</v>
+      </c>
       <c r="AE77" s="3"/>
       <c r="AF77" s="3"/>
       <c r="AG77" s="3"/>
@@ -8289,8 +8629,12 @@
       <c r="AB78" s="2">
         <v>152</v>
       </c>
-      <c r="AC78" s="3"/>
-      <c r="AD78" s="3"/>
+      <c r="AC78" s="2">
+        <v>236</v>
+      </c>
+      <c r="AD78" s="3">
+        <v>278</v>
+      </c>
       <c r="AE78" s="3"/>
       <c r="AF78" s="3"/>
       <c r="AG78" s="3"/>
@@ -8384,8 +8728,12 @@
       <c r="AB79" s="2">
         <v>1138</v>
       </c>
-      <c r="AC79" s="3"/>
-      <c r="AD79" s="3"/>
+      <c r="AC79" s="2">
+        <v>1246</v>
+      </c>
+      <c r="AD79" s="3">
+        <v>1287</v>
+      </c>
       <c r="AE79" s="3"/>
       <c r="AF79" s="3"/>
       <c r="AG79" s="3"/>
@@ -8479,8 +8827,12 @@
       <c r="AB80" s="2">
         <v>215</v>
       </c>
-      <c r="AC80" s="3"/>
-      <c r="AD80" s="3"/>
+      <c r="AC80" s="2">
+        <v>246</v>
+      </c>
+      <c r="AD80" s="3">
+        <v>263</v>
+      </c>
       <c r="AE80" s="3"/>
       <c r="AF80" s="3"/>
       <c r="AG80" s="3"/>
@@ -8574,8 +8926,12 @@
       <c r="AB81" s="2">
         <v>249</v>
       </c>
-      <c r="AC81" s="3"/>
-      <c r="AD81" s="3"/>
+      <c r="AC81" s="2">
+        <v>283</v>
+      </c>
+      <c r="AD81" s="3">
+        <v>296</v>
+      </c>
       <c r="AE81" s="3"/>
       <c r="AF81" s="3"/>
       <c r="AG81" s="3"/>
@@ -8669,8 +9025,12 @@
       <c r="AB82" s="2">
         <v>283</v>
       </c>
-      <c r="AC82" s="3"/>
-      <c r="AD82" s="3"/>
+      <c r="AC82" s="2">
+        <v>316</v>
+      </c>
+      <c r="AD82" s="3">
+        <v>353</v>
+      </c>
       <c r="AE82" s="3"/>
       <c r="AF82" s="3"/>
       <c r="AG82" s="3"/>
@@ -8764,8 +9124,12 @@
       <c r="AB83" s="2">
         <v>183</v>
       </c>
-      <c r="AC83" s="3"/>
-      <c r="AD83" s="3"/>
+      <c r="AC83" s="2">
+        <v>204</v>
+      </c>
+      <c r="AD83" s="3">
+        <v>215</v>
+      </c>
       <c r="AE83" s="3"/>
       <c r="AF83" s="3"/>
       <c r="AG83" s="3"/>
@@ -8859,8 +9223,12 @@
       <c r="AB84" s="2">
         <v>309</v>
       </c>
-      <c r="AC84" s="3"/>
-      <c r="AD84" s="3"/>
+      <c r="AC84" s="2">
+        <v>340</v>
+      </c>
+      <c r="AD84" s="3">
+        <v>359</v>
+      </c>
       <c r="AE84" s="3"/>
       <c r="AF84" s="3"/>
       <c r="AG84" s="3"/>
@@ -8954,8 +9322,12 @@
       <c r="AB85" s="2">
         <v>275</v>
       </c>
-      <c r="AC85" s="3"/>
-      <c r="AD85" s="3"/>
+      <c r="AC85" s="2">
+        <v>294</v>
+      </c>
+      <c r="AD85" s="3">
+        <v>304</v>
+      </c>
       <c r="AE85" s="3"/>
       <c r="AF85" s="3"/>
       <c r="AG85" s="3"/>
@@ -9049,8 +9421,12 @@
       <c r="AB86" s="2">
         <v>170</v>
       </c>
-      <c r="AC86" s="3"/>
-      <c r="AD86" s="3"/>
+      <c r="AC86" s="2">
+        <v>185</v>
+      </c>
+      <c r="AD86" s="3">
+        <v>204</v>
+      </c>
       <c r="AE86" s="3"/>
       <c r="AF86" s="3"/>
       <c r="AG86" s="3"/>
@@ -9144,8 +9520,12 @@
       <c r="AB87" s="2">
         <v>69</v>
       </c>
-      <c r="AC87" s="3"/>
-      <c r="AD87" s="3"/>
+      <c r="AC87" s="2">
+        <v>89</v>
+      </c>
+      <c r="AD87" s="3">
+        <v>94</v>
+      </c>
       <c r="AE87" s="3"/>
       <c r="AF87" s="3"/>
       <c r="AG87" s="3"/>
@@ -9239,8 +9619,12 @@
       <c r="AB88" s="2">
         <v>153</v>
       </c>
-      <c r="AC88" s="3"/>
-      <c r="AD88" s="3"/>
+      <c r="AC88" s="2">
+        <v>185</v>
+      </c>
+      <c r="AD88" s="3">
+        <v>198</v>
+      </c>
       <c r="AE88" s="3"/>
       <c r="AF88" s="3"/>
       <c r="AG88" s="3"/>
@@ -9334,8 +9718,12 @@
       <c r="AB89" s="2">
         <v>272</v>
       </c>
-      <c r="AC89" s="3"/>
-      <c r="AD89" s="3"/>
+      <c r="AC89" s="2">
+        <v>296</v>
+      </c>
+      <c r="AD89" s="3">
+        <v>325</v>
+      </c>
       <c r="AE89" s="3"/>
       <c r="AF89" s="3"/>
       <c r="AG89" s="3"/>
@@ -9429,8 +9817,12 @@
       <c r="AB90" s="2">
         <v>128</v>
       </c>
-      <c r="AC90" s="3"/>
-      <c r="AD90" s="3"/>
+      <c r="AC90" s="2">
+        <v>153</v>
+      </c>
+      <c r="AD90" s="3">
+        <v>162</v>
+      </c>
       <c r="AE90" s="3"/>
       <c r="AF90" s="3"/>
       <c r="AG90" s="3"/>
@@ -9524,8 +9916,12 @@
       <c r="AB91" s="2">
         <v>108</v>
       </c>
-      <c r="AC91" s="3"/>
-      <c r="AD91" s="3"/>
+      <c r="AC91" s="2">
+        <v>168</v>
+      </c>
+      <c r="AD91" s="3">
+        <v>180</v>
+      </c>
       <c r="AE91" s="3"/>
       <c r="AF91" s="3"/>
       <c r="AG91" s="3"/>
@@ -9619,8 +10015,12 @@
       <c r="AB92" s="2">
         <v>183</v>
       </c>
-      <c r="AC92" s="3"/>
-      <c r="AD92" s="3"/>
+      <c r="AC92" s="2">
+        <v>209</v>
+      </c>
+      <c r="AD92" s="3">
+        <v>211</v>
+      </c>
       <c r="AE92" s="3"/>
       <c r="AF92" s="3"/>
       <c r="AG92" s="3"/>
@@ -9714,8 +10114,12 @@
       <c r="AB93" s="2">
         <v>589</v>
       </c>
-      <c r="AC93" s="3"/>
-      <c r="AD93" s="3"/>
+      <c r="AC93" s="2">
+        <v>645</v>
+      </c>
+      <c r="AD93" s="3">
+        <v>666</v>
+      </c>
       <c r="AE93" s="3"/>
       <c r="AF93" s="3"/>
       <c r="AG93" s="3"/>
@@ -9809,8 +10213,12 @@
       <c r="AB94" s="2">
         <v>221</v>
       </c>
-      <c r="AC94" s="3"/>
-      <c r="AD94" s="3"/>
+      <c r="AC94" s="2">
+        <v>242</v>
+      </c>
+      <c r="AD94" s="3">
+        <v>250</v>
+      </c>
       <c r="AE94" s="3"/>
       <c r="AF94" s="3"/>
       <c r="AG94" s="3"/>
@@ -9904,8 +10312,12 @@
       <c r="AB95" s="2">
         <v>663</v>
       </c>
-      <c r="AC95" s="3"/>
-      <c r="AD95" s="3"/>
+      <c r="AC95" s="2">
+        <v>728</v>
+      </c>
+      <c r="AD95" s="3">
+        <v>759</v>
+      </c>
       <c r="AE95" s="3"/>
       <c r="AF95" s="3"/>
       <c r="AG95" s="3"/>
@@ -9999,8 +10411,12 @@
       <c r="AB96" s="2">
         <v>434</v>
       </c>
-      <c r="AC96" s="3"/>
-      <c r="AD96" s="3"/>
+      <c r="AC96" s="2">
+        <v>489</v>
+      </c>
+      <c r="AD96" s="3">
+        <v>521</v>
+      </c>
       <c r="AE96" s="3"/>
       <c r="AF96" s="3"/>
       <c r="AG96" s="3"/>
@@ -10094,8 +10510,12 @@
       <c r="AB97" s="2">
         <v>263</v>
       </c>
-      <c r="AC97" s="3"/>
-      <c r="AD97" s="3"/>
+      <c r="AC97" s="2">
+        <v>289</v>
+      </c>
+      <c r="AD97" s="3">
+        <v>298</v>
+      </c>
       <c r="AE97" s="3"/>
       <c r="AF97" s="3"/>
       <c r="AG97" s="3"/>
@@ -10189,8 +10609,12 @@
       <c r="AB98" s="2">
         <v>515</v>
       </c>
-      <c r="AC98" s="3"/>
-      <c r="AD98" s="3"/>
+      <c r="AC98" s="2">
+        <v>558</v>
+      </c>
+      <c r="AD98" s="3">
+        <v>620</v>
+      </c>
       <c r="AE98" s="3"/>
       <c r="AF98" s="3"/>
       <c r="AG98" s="3"/>
@@ -10284,8 +10708,12 @@
       <c r="AB99" s="2">
         <v>445</v>
       </c>
-      <c r="AC99" s="3"/>
-      <c r="AD99" s="3"/>
+      <c r="AC99" s="2">
+        <v>489</v>
+      </c>
+      <c r="AD99" s="3">
+        <v>503</v>
+      </c>
       <c r="AE99" s="3"/>
       <c r="AF99" s="3"/>
       <c r="AG99" s="3"/>
@@ -10379,8 +10807,12 @@
       <c r="AB100" s="2">
         <v>300</v>
       </c>
-      <c r="AC100" s="3"/>
-      <c r="AD100" s="3"/>
+      <c r="AC100" s="2">
+        <v>333</v>
+      </c>
+      <c r="AD100" s="3">
+        <v>350</v>
+      </c>
       <c r="AE100" s="3"/>
       <c r="AF100" s="3"/>
       <c r="AG100" s="3"/>
@@ -10474,8 +10906,12 @@
       <c r="AB101" s="2">
         <v>283</v>
       </c>
-      <c r="AC101" s="3"/>
-      <c r="AD101" s="3"/>
+      <c r="AC101" s="2">
+        <v>318</v>
+      </c>
+      <c r="AD101" s="3">
+        <v>322</v>
+      </c>
       <c r="AE101" s="3"/>
       <c r="AF101" s="3"/>
       <c r="AG101" s="3"/>
@@ -10569,8 +11005,12 @@
       <c r="AB102" s="2">
         <v>304</v>
       </c>
-      <c r="AC102" s="3"/>
-      <c r="AD102" s="3"/>
+      <c r="AC102" s="2">
+        <v>345</v>
+      </c>
+      <c r="AD102" s="3">
+        <v>362</v>
+      </c>
       <c r="AE102" s="3"/>
       <c r="AF102" s="3"/>
       <c r="AG102" s="3"/>
@@ -10664,8 +11104,12 @@
       <c r="AB103" s="2">
         <v>230</v>
       </c>
-      <c r="AC103" s="3"/>
-      <c r="AD103" s="3"/>
+      <c r="AC103" s="2">
+        <v>252</v>
+      </c>
+      <c r="AD103" s="3">
+        <v>266</v>
+      </c>
       <c r="AE103" s="3"/>
       <c r="AF103" s="3"/>
       <c r="AG103" s="3"/>
@@ -10759,8 +11203,12 @@
       <c r="AB104" s="2">
         <v>246</v>
       </c>
-      <c r="AC104" s="3"/>
-      <c r="AD104" s="3"/>
+      <c r="AC104" s="2">
+        <v>277</v>
+      </c>
+      <c r="AD104" s="3">
+        <v>285</v>
+      </c>
       <c r="AE104" s="3"/>
       <c r="AF104" s="3"/>
       <c r="AG104" s="3"/>
@@ -10854,8 +11302,12 @@
       <c r="AB105" s="2">
         <v>422</v>
       </c>
-      <c r="AC105" s="3"/>
-      <c r="AD105" s="3"/>
+      <c r="AC105" s="2">
+        <v>450</v>
+      </c>
+      <c r="AD105" s="3">
+        <v>469</v>
+      </c>
       <c r="AE105" s="3"/>
       <c r="AF105" s="3"/>
       <c r="AG105" s="3"/>
@@ -10949,8 +11401,12 @@
       <c r="AB106" s="2">
         <v>194</v>
       </c>
-      <c r="AC106" s="3"/>
-      <c r="AD106" s="3"/>
+      <c r="AC106" s="2">
+        <v>232</v>
+      </c>
+      <c r="AD106" s="3">
+        <v>248</v>
+      </c>
       <c r="AE106" s="3"/>
       <c r="AF106" s="3"/>
       <c r="AG106" s="3"/>
@@ -11044,8 +11500,12 @@
       <c r="AB107" s="2">
         <v>295</v>
       </c>
-      <c r="AC107" s="3"/>
-      <c r="AD107" s="3"/>
+      <c r="AC107" s="2">
+        <v>317</v>
+      </c>
+      <c r="AD107" s="3">
+        <v>348</v>
+      </c>
       <c r="AE107" s="3"/>
       <c r="AF107" s="3"/>
       <c r="AG107" s="3"/>
@@ -11139,8 +11599,12 @@
       <c r="AB108" s="2">
         <v>285</v>
       </c>
-      <c r="AC108" s="3"/>
-      <c r="AD108" s="3"/>
+      <c r="AC108" s="2">
+        <v>323</v>
+      </c>
+      <c r="AD108" s="3">
+        <v>338</v>
+      </c>
       <c r="AE108" s="3"/>
       <c r="AF108" s="3"/>
       <c r="AG108" s="3"/>
@@ -11234,8 +11698,12 @@
       <c r="AB109" s="2">
         <v>226</v>
       </c>
-      <c r="AC109" s="3"/>
-      <c r="AD109" s="3"/>
+      <c r="AC109" s="2">
+        <v>248</v>
+      </c>
+      <c r="AD109" s="3">
+        <v>257</v>
+      </c>
       <c r="AE109" s="3"/>
       <c r="AF109" s="3"/>
       <c r="AG109" s="3"/>
@@ -11329,8 +11797,12 @@
       <c r="AB110" s="2">
         <v>240</v>
       </c>
-      <c r="AC110" s="3"/>
-      <c r="AD110" s="3"/>
+      <c r="AC110" s="2">
+        <v>258</v>
+      </c>
+      <c r="AD110" s="3">
+        <v>272</v>
+      </c>
       <c r="AE110" s="3"/>
       <c r="AF110" s="3"/>
       <c r="AG110" s="3"/>
@@ -11424,8 +11896,12 @@
       <c r="AB111" s="2">
         <v>144</v>
       </c>
-      <c r="AC111" s="3"/>
-      <c r="AD111" s="3"/>
+      <c r="AC111" s="2">
+        <v>156</v>
+      </c>
+      <c r="AD111" s="3">
+        <v>169</v>
+      </c>
       <c r="AE111" s="3"/>
       <c r="AF111" s="3"/>
       <c r="AG111" s="3"/>
@@ -11519,8 +11995,12 @@
       <c r="AB112" s="2">
         <v>577</v>
       </c>
-      <c r="AC112" s="3"/>
-      <c r="AD112" s="3"/>
+      <c r="AC112" s="2">
+        <v>631</v>
+      </c>
+      <c r="AD112" s="3">
+        <v>671</v>
+      </c>
       <c r="AE112" s="3"/>
       <c r="AF112" s="3"/>
       <c r="AG112" s="3"/>
@@ -11614,8 +12094,12 @@
       <c r="AB113" s="2">
         <v>408</v>
       </c>
-      <c r="AC113" s="3"/>
-      <c r="AD113" s="3"/>
+      <c r="AC113" s="2">
+        <v>477</v>
+      </c>
+      <c r="AD113" s="3">
+        <v>490</v>
+      </c>
       <c r="AE113" s="3"/>
       <c r="AF113" s="3"/>
       <c r="AG113" s="3"/>
@@ -11709,8 +12193,12 @@
       <c r="AB114" s="2">
         <v>271</v>
       </c>
-      <c r="AC114" s="3"/>
-      <c r="AD114" s="3"/>
+      <c r="AC114" s="2">
+        <v>293</v>
+      </c>
+      <c r="AD114" s="3">
+        <v>316</v>
+      </c>
       <c r="AE114" s="3"/>
       <c r="AF114" s="3"/>
       <c r="AG114" s="3"/>
@@ -11804,8 +12292,12 @@
       <c r="AB115" s="2">
         <v>412</v>
       </c>
-      <c r="AC115" s="3"/>
-      <c r="AD115" s="3"/>
+      <c r="AC115" s="2">
+        <v>493</v>
+      </c>
+      <c r="AD115" s="3">
+        <v>530</v>
+      </c>
       <c r="AE115" s="3"/>
       <c r="AF115" s="3"/>
       <c r="AG115" s="3"/>
@@ -11899,8 +12391,12 @@
       <c r="AB116" s="2">
         <v>252</v>
       </c>
-      <c r="AC116" s="3"/>
-      <c r="AD116" s="3"/>
+      <c r="AC116" s="2">
+        <v>299</v>
+      </c>
+      <c r="AD116" s="3">
+        <v>311</v>
+      </c>
       <c r="AE116" s="3"/>
       <c r="AF116" s="3"/>
       <c r="AG116" s="3"/>
@@ -11994,8 +12490,12 @@
       <c r="AB117" s="2">
         <v>175</v>
       </c>
-      <c r="AC117" s="3"/>
-      <c r="AD117" s="3"/>
+      <c r="AC117" s="2">
+        <v>189</v>
+      </c>
+      <c r="AD117" s="3">
+        <v>200</v>
+      </c>
       <c r="AE117" s="3"/>
       <c r="AF117" s="3"/>
       <c r="AG117" s="3"/>
@@ -12089,8 +12589,12 @@
       <c r="AB118" s="2">
         <v>586</v>
       </c>
-      <c r="AC118" s="3"/>
-      <c r="AD118" s="3"/>
+      <c r="AC118" s="2">
+        <v>648</v>
+      </c>
+      <c r="AD118" s="3">
+        <v>685</v>
+      </c>
       <c r="AE118" s="3"/>
       <c r="AF118" s="3"/>
       <c r="AG118" s="3"/>
@@ -12184,8 +12688,12 @@
       <c r="AB119" s="2">
         <v>208</v>
       </c>
-      <c r="AC119" s="3"/>
-      <c r="AD119" s="3"/>
+      <c r="AC119" s="2">
+        <v>232</v>
+      </c>
+      <c r="AD119" s="3">
+        <v>262</v>
+      </c>
       <c r="AE119" s="3"/>
       <c r="AF119" s="3"/>
       <c r="AG119" s="3"/>
@@ -12279,8 +12787,12 @@
       <c r="AB120" s="2">
         <v>288</v>
       </c>
-      <c r="AC120" s="3"/>
-      <c r="AD120" s="3"/>
+      <c r="AC120" s="2">
+        <v>339</v>
+      </c>
+      <c r="AD120" s="3">
+        <v>359</v>
+      </c>
       <c r="AE120" s="3"/>
       <c r="AF120" s="3"/>
       <c r="AG120" s="3"/>
@@ -12374,8 +12886,12 @@
       <c r="AB121" s="2">
         <v>313</v>
       </c>
-      <c r="AC121" s="3"/>
-      <c r="AD121" s="3"/>
+      <c r="AC121" s="2">
+        <v>364</v>
+      </c>
+      <c r="AD121" s="3">
+        <v>389</v>
+      </c>
       <c r="AE121" s="3"/>
       <c r="AF121" s="3"/>
       <c r="AG121" s="3"/>
@@ -12469,8 +12985,12 @@
       <c r="AB122" s="2">
         <v>454</v>
       </c>
-      <c r="AC122" s="3"/>
-      <c r="AD122" s="3"/>
+      <c r="AC122" s="2">
+        <v>492</v>
+      </c>
+      <c r="AD122" s="3">
+        <v>526</v>
+      </c>
       <c r="AE122" s="3"/>
       <c r="AF122" s="3"/>
       <c r="AG122" s="3"/>
@@ -12564,8 +13084,12 @@
       <c r="AB123" s="2">
         <v>338</v>
       </c>
-      <c r="AC123" s="3"/>
-      <c r="AD123" s="3"/>
+      <c r="AC123" s="2">
+        <v>363</v>
+      </c>
+      <c r="AD123" s="3">
+        <v>383</v>
+      </c>
       <c r="AE123" s="3"/>
       <c r="AF123" s="3"/>
       <c r="AG123" s="3"/>
@@ -12659,8 +13183,12 @@
       <c r="AB124" s="2">
         <v>255</v>
       </c>
-      <c r="AC124" s="3"/>
-      <c r="AD124" s="3"/>
+      <c r="AC124" s="2">
+        <v>268</v>
+      </c>
+      <c r="AD124" s="3">
+        <v>300</v>
+      </c>
       <c r="AE124" s="3"/>
       <c r="AF124" s="3"/>
       <c r="AG124" s="3"/>
@@ -12754,8 +13282,12 @@
       <c r="AB125" s="2">
         <v>191</v>
       </c>
-      <c r="AC125" s="3"/>
-      <c r="AD125" s="3"/>
+      <c r="AC125" s="2">
+        <v>212</v>
+      </c>
+      <c r="AD125" s="3">
+        <v>222</v>
+      </c>
       <c r="AE125" s="3"/>
       <c r="AF125" s="3"/>
       <c r="AG125" s="3"/>
@@ -12849,8 +13381,12 @@
       <c r="AB126" s="2">
         <v>629</v>
       </c>
-      <c r="AC126" s="3"/>
-      <c r="AD126" s="3"/>
+      <c r="AC126" s="2">
+        <v>698</v>
+      </c>
+      <c r="AD126" s="3">
+        <v>753</v>
+      </c>
       <c r="AE126" s="3"/>
       <c r="AF126" s="3"/>
       <c r="AG126" s="3"/>
@@ -12944,8 +13480,12 @@
       <c r="AB127" s="2">
         <v>398</v>
       </c>
-      <c r="AC127" s="3"/>
-      <c r="AD127" s="3"/>
+      <c r="AC127" s="2">
+        <v>452</v>
+      </c>
+      <c r="AD127" s="3">
+        <v>494</v>
+      </c>
       <c r="AE127" s="3"/>
       <c r="AF127" s="3"/>
       <c r="AG127" s="3"/>
@@ -13039,8 +13579,12 @@
       <c r="AB128" s="2">
         <v>181</v>
       </c>
-      <c r="AC128" s="3"/>
-      <c r="AD128" s="3"/>
+      <c r="AC128" s="2">
+        <v>207</v>
+      </c>
+      <c r="AD128" s="3">
+        <v>229</v>
+      </c>
       <c r="AE128" s="3"/>
       <c r="AF128" s="3"/>
       <c r="AG128" s="3"/>
@@ -13134,8 +13678,12 @@
       <c r="AB129" s="2">
         <v>132</v>
       </c>
-      <c r="AC129" s="3"/>
-      <c r="AD129" s="3"/>
+      <c r="AC129" s="2">
+        <v>155</v>
+      </c>
+      <c r="AD129" s="3">
+        <v>161</v>
+      </c>
       <c r="AE129" s="3"/>
       <c r="AF129" s="3"/>
       <c r="AG129" s="3"/>
@@ -13229,8 +13777,12 @@
       <c r="AB130" s="2">
         <v>597</v>
       </c>
-      <c r="AC130" s="3"/>
-      <c r="AD130" s="3"/>
+      <c r="AC130" s="2">
+        <v>792</v>
+      </c>
+      <c r="AD130" s="3">
+        <v>858</v>
+      </c>
       <c r="AE130" s="3"/>
       <c r="AF130" s="3"/>
       <c r="AG130" s="3"/>
@@ -13324,8 +13876,12 @@
       <c r="AB131" s="2">
         <v>258</v>
       </c>
-      <c r="AC131" s="3"/>
-      <c r="AD131" s="3"/>
+      <c r="AC131" s="2">
+        <v>281</v>
+      </c>
+      <c r="AD131" s="3">
+        <v>306</v>
+      </c>
       <c r="AE131" s="3"/>
       <c r="AF131" s="3"/>
       <c r="AG131" s="3"/>
@@ -13419,8 +13975,12 @@
       <c r="AB132" s="2">
         <v>809</v>
       </c>
-      <c r="AC132" s="3"/>
-      <c r="AD132" s="3"/>
+      <c r="AC132" s="2">
+        <v>876</v>
+      </c>
+      <c r="AD132" s="3">
+        <v>921</v>
+      </c>
       <c r="AE132" s="3"/>
       <c r="AF132" s="3"/>
       <c r="AG132" s="3"/>
@@ -13514,8 +14074,12 @@
       <c r="AB133" s="2">
         <v>692</v>
       </c>
-      <c r="AC133" s="3"/>
-      <c r="AD133" s="3"/>
+      <c r="AC133" s="2">
+        <v>833</v>
+      </c>
+      <c r="AD133" s="3">
+        <v>870</v>
+      </c>
       <c r="AE133" s="3"/>
       <c r="AF133" s="3"/>
       <c r="AG133" s="3"/>
@@ -13609,8 +14173,12 @@
       <c r="AB134" s="2">
         <v>704</v>
       </c>
-      <c r="AC134" s="3"/>
-      <c r="AD134" s="3"/>
+      <c r="AC134" s="2">
+        <v>755</v>
+      </c>
+      <c r="AD134" s="3">
+        <v>791</v>
+      </c>
       <c r="AE134" s="3"/>
       <c r="AF134" s="3"/>
       <c r="AG134" s="3"/>
@@ -13704,8 +14272,12 @@
       <c r="AB135" s="2">
         <v>642</v>
       </c>
-      <c r="AC135" s="3"/>
-      <c r="AD135" s="3"/>
+      <c r="AC135" s="2">
+        <v>726</v>
+      </c>
+      <c r="AD135" s="3">
+        <v>838</v>
+      </c>
       <c r="AE135" s="3"/>
       <c r="AF135" s="3"/>
       <c r="AG135" s="3"/>
@@ -13799,8 +14371,12 @@
       <c r="AB136" s="2">
         <v>277</v>
       </c>
-      <c r="AC136" s="3"/>
-      <c r="AD136" s="3"/>
+      <c r="AC136" s="2">
+        <v>311</v>
+      </c>
+      <c r="AD136" s="3">
+        <v>338</v>
+      </c>
       <c r="AE136" s="3"/>
       <c r="AF136" s="3"/>
       <c r="AG136" s="3"/>
@@ -13894,8 +14470,12 @@
       <c r="AB137" s="2">
         <v>223</v>
       </c>
-      <c r="AC137" s="3"/>
-      <c r="AD137" s="3"/>
+      <c r="AC137" s="2">
+        <v>252</v>
+      </c>
+      <c r="AD137" s="3">
+        <v>275</v>
+      </c>
       <c r="AE137" s="3"/>
       <c r="AF137" s="3"/>
       <c r="AG137" s="3"/>
@@ -13989,8 +14569,12 @@
       <c r="AB138" s="2">
         <v>254</v>
       </c>
-      <c r="AC138" s="3"/>
-      <c r="AD138" s="3"/>
+      <c r="AC138" s="2">
+        <v>279</v>
+      </c>
+      <c r="AD138" s="3">
+        <v>301</v>
+      </c>
       <c r="AE138" s="3"/>
       <c r="AF138" s="3"/>
       <c r="AG138" s="3"/>
@@ -14084,8 +14668,12 @@
       <c r="AB139" s="2">
         <v>302</v>
       </c>
-      <c r="AC139" s="3"/>
-      <c r="AD139" s="3"/>
+      <c r="AC139" s="2">
+        <v>343</v>
+      </c>
+      <c r="AD139" s="3">
+        <v>428</v>
+      </c>
       <c r="AE139" s="3"/>
       <c r="AF139" s="3"/>
       <c r="AG139" s="3"/>
@@ -14179,8 +14767,12 @@
       <c r="AB140" s="2">
         <v>218</v>
       </c>
-      <c r="AC140" s="3"/>
-      <c r="AD140" s="3"/>
+      <c r="AC140" s="2">
+        <v>243</v>
+      </c>
+      <c r="AD140" s="3">
+        <v>269</v>
+      </c>
       <c r="AE140" s="3"/>
       <c r="AF140" s="3"/>
       <c r="AG140" s="3"/>
@@ -14274,8 +14866,12 @@
       <c r="AB141" s="2">
         <v>357</v>
       </c>
-      <c r="AC141" s="3"/>
-      <c r="AD141" s="3"/>
+      <c r="AC141" s="2">
+        <v>413</v>
+      </c>
+      <c r="AD141" s="3">
+        <v>425</v>
+      </c>
       <c r="AE141" s="3"/>
       <c r="AF141" s="3"/>
       <c r="AG141" s="3"/>
@@ -14369,8 +14965,12 @@
       <c r="AB142" s="2">
         <v>356</v>
       </c>
-      <c r="AC142" s="3"/>
-      <c r="AD142" s="3"/>
+      <c r="AC142" s="2">
+        <v>411</v>
+      </c>
+      <c r="AD142" s="3">
+        <v>450</v>
+      </c>
       <c r="AE142" s="3"/>
       <c r="AF142" s="3"/>
       <c r="AG142" s="3"/>
@@ -14464,8 +15064,12 @@
       <c r="AB143" s="2">
         <v>76</v>
       </c>
-      <c r="AC143" s="3"/>
-      <c r="AD143" s="3"/>
+      <c r="AC143" s="2">
+        <v>99</v>
+      </c>
+      <c r="AD143" s="3">
+        <v>114</v>
+      </c>
       <c r="AE143" s="3"/>
       <c r="AF143" s="3"/>
       <c r="AG143" s="3"/>
@@ -14559,8 +15163,12 @@
       <c r="AB144" s="2">
         <v>470</v>
       </c>
-      <c r="AC144" s="3"/>
-      <c r="AD144" s="3"/>
+      <c r="AC144" s="2">
+        <v>534</v>
+      </c>
+      <c r="AD144" s="3">
+        <v>570</v>
+      </c>
       <c r="AE144" s="3"/>
       <c r="AF144" s="3"/>
       <c r="AG144" s="3"/>
@@ -14654,8 +15262,12 @@
       <c r="AB145" s="2">
         <v>191</v>
       </c>
-      <c r="AC145" s="3"/>
-      <c r="AD145" s="3"/>
+      <c r="AC145" s="2">
+        <v>231</v>
+      </c>
+      <c r="AD145" s="3">
+        <v>243</v>
+      </c>
       <c r="AE145" s="3"/>
       <c r="AF145" s="3"/>
       <c r="AG145" s="3"/>
@@ -14749,8 +15361,12 @@
       <c r="AB146" s="2">
         <v>736</v>
       </c>
-      <c r="AC146" s="3"/>
-      <c r="AD146" s="3"/>
+      <c r="AC146" s="2">
+        <v>811</v>
+      </c>
+      <c r="AD146" s="3">
+        <v>887</v>
+      </c>
       <c r="AE146" s="3"/>
       <c r="AF146" s="3"/>
       <c r="AG146" s="3"/>
@@ -14844,8 +15460,12 @@
       <c r="AB147" s="2">
         <v>302</v>
       </c>
-      <c r="AC147" s="3"/>
-      <c r="AD147" s="3"/>
+      <c r="AC147" s="2">
+        <v>334</v>
+      </c>
+      <c r="AD147" s="3">
+        <v>361</v>
+      </c>
       <c r="AE147" s="3"/>
       <c r="AF147" s="3"/>
       <c r="AG147" s="3"/>
@@ -14939,8 +15559,12 @@
       <c r="AB148" s="2">
         <v>216</v>
       </c>
-      <c r="AC148" s="3"/>
-      <c r="AD148" s="3"/>
+      <c r="AC148" s="2">
+        <v>220</v>
+      </c>
+      <c r="AD148" s="3">
+        <v>224</v>
+      </c>
       <c r="AE148" s="3"/>
       <c r="AF148" s="3"/>
       <c r="AG148" s="3"/>
@@ -15034,8 +15658,12 @@
       <c r="AB149" s="2">
         <v>321</v>
       </c>
-      <c r="AC149" s="3"/>
-      <c r="AD149" s="3"/>
+      <c r="AC149" s="2">
+        <v>350</v>
+      </c>
+      <c r="AD149" s="3">
+        <v>394</v>
+      </c>
       <c r="AE149" s="3"/>
       <c r="AF149" s="3"/>
       <c r="AG149" s="3"/>
@@ -15043,6 +15671,9 @@
       <c r="AI149" s="3"/>
       <c r="AJ149" s="3"/>
       <c r="AK149" s="3"/>
+    </row>
+    <row r="150" spans="1:37">
+      <c r="AC150" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated as of 04/06
</commit_message>
<xml_diff>
--- a/covid_data.xlsx
+++ b/covid_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
+    <workbookView xWindow="5900" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -472,7 +472,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -529,38 +539,79 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="60">
+    <cellStyle name="Comma" xfId="21" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -571,6 +622,25 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -581,6 +651,25 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -912,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AD149"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AI24" sqref="AI24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1012,10 +1101,16 @@
       <c r="AD1" s="3">
         <v>33</v>
       </c>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
-      <c r="AG1" s="3"/>
-      <c r="AH1" s="3"/>
+      <c r="AE1" s="2">
+        <v>36</v>
+      </c>
+      <c r="AF1" s="4">
+        <v>49</v>
+      </c>
+      <c r="AG1" s="4">
+        <v>64</v>
+      </c>
+      <c r="AH1" s="4"/>
       <c r="AI1" s="3"/>
       <c r="AJ1" s="3"/>
       <c r="AK1" s="3"/>
@@ -1111,10 +1206,16 @@
       <c r="AD2" s="3">
         <v>151</v>
       </c>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
-      <c r="AG2" s="3"/>
-      <c r="AH2" s="3"/>
+      <c r="AE2" s="2">
+        <v>169</v>
+      </c>
+      <c r="AF2" s="4">
+        <v>196</v>
+      </c>
+      <c r="AG2" s="4">
+        <v>235</v>
+      </c>
+      <c r="AH2" s="4"/>
       <c r="AI2" s="3"/>
       <c r="AJ2" s="3"/>
       <c r="AK2" s="3"/>
@@ -1210,10 +1311,16 @@
       <c r="AD3" s="3">
         <v>100</v>
       </c>
-      <c r="AE3" s="3"/>
-      <c r="AF3" s="3"/>
-      <c r="AG3" s="3"/>
-      <c r="AH3" s="3"/>
+      <c r="AE3" s="2">
+        <v>112</v>
+      </c>
+      <c r="AF3" s="4">
+        <v>119</v>
+      </c>
+      <c r="AG3" s="4">
+        <v>139</v>
+      </c>
+      <c r="AH3" s="4"/>
       <c r="AI3" s="3"/>
       <c r="AJ3" s="3"/>
       <c r="AK3" s="3"/>
@@ -1309,10 +1416,16 @@
       <c r="AD4" s="3">
         <v>117</v>
       </c>
-      <c r="AE4" s="3"/>
-      <c r="AF4" s="3"/>
-      <c r="AG4" s="3"/>
-      <c r="AH4" s="3"/>
+      <c r="AE4" s="2">
+        <v>123</v>
+      </c>
+      <c r="AF4" s="4">
+        <v>143</v>
+      </c>
+      <c r="AG4" s="4">
+        <v>173</v>
+      </c>
+      <c r="AH4" s="4"/>
       <c r="AI4" s="3"/>
       <c r="AJ4" s="3"/>
       <c r="AK4" s="3"/>
@@ -1408,10 +1521,16 @@
       <c r="AD5" s="3">
         <v>52</v>
       </c>
-      <c r="AE5" s="3"/>
-      <c r="AF5" s="3"/>
-      <c r="AG5" s="3"/>
-      <c r="AH5" s="3"/>
+      <c r="AE5" s="2">
+        <v>55</v>
+      </c>
+      <c r="AF5" s="4">
+        <v>77</v>
+      </c>
+      <c r="AG5" s="4">
+        <v>109</v>
+      </c>
+      <c r="AH5" s="4"/>
       <c r="AI5" s="3"/>
       <c r="AJ5" s="3"/>
       <c r="AK5" s="3"/>
@@ -1507,10 +1626,16 @@
       <c r="AD6" s="3">
         <v>95</v>
       </c>
-      <c r="AE6" s="3"/>
-      <c r="AF6" s="3"/>
-      <c r="AG6" s="3"/>
-      <c r="AH6" s="3"/>
+      <c r="AE6" s="2">
+        <v>107</v>
+      </c>
+      <c r="AF6" s="4">
+        <v>127</v>
+      </c>
+      <c r="AG6" s="4">
+        <v>159</v>
+      </c>
+      <c r="AH6" s="4"/>
       <c r="AI6" s="3"/>
       <c r="AJ6" s="3"/>
       <c r="AK6" s="3"/>
@@ -1606,10 +1731,16 @@
       <c r="AD7" s="3">
         <v>138</v>
       </c>
-      <c r="AE7" s="3"/>
-      <c r="AF7" s="3"/>
-      <c r="AG7" s="3"/>
-      <c r="AH7" s="3"/>
+      <c r="AE7" s="2">
+        <v>162</v>
+      </c>
+      <c r="AF7" s="4">
+        <v>182</v>
+      </c>
+      <c r="AG7" s="4">
+        <v>241</v>
+      </c>
+      <c r="AH7" s="4"/>
       <c r="AI7" s="3"/>
       <c r="AJ7" s="3"/>
       <c r="AK7" s="3"/>
@@ -1705,10 +1836,16 @@
       <c r="AD8" s="3">
         <v>71</v>
       </c>
-      <c r="AE8" s="3"/>
-      <c r="AF8" s="3"/>
-      <c r="AG8" s="3"/>
-      <c r="AH8" s="3"/>
+      <c r="AE8" s="2">
+        <v>86</v>
+      </c>
+      <c r="AF8" s="4">
+        <v>92</v>
+      </c>
+      <c r="AG8" s="4">
+        <v>106</v>
+      </c>
+      <c r="AH8" s="4"/>
       <c r="AI8" s="3"/>
       <c r="AJ8" s="3"/>
       <c r="AK8" s="3"/>
@@ -1804,10 +1941,16 @@
       <c r="AD9" s="3">
         <v>72</v>
       </c>
-      <c r="AE9" s="3"/>
-      <c r="AF9" s="3"/>
-      <c r="AG9" s="3"/>
-      <c r="AH9" s="3"/>
+      <c r="AE9" s="2">
+        <v>85</v>
+      </c>
+      <c r="AF9" s="4">
+        <v>94</v>
+      </c>
+      <c r="AG9" s="4">
+        <v>108</v>
+      </c>
+      <c r="AH9" s="4"/>
       <c r="AI9" s="3"/>
       <c r="AJ9" s="3"/>
       <c r="AK9" s="3"/>
@@ -1903,10 +2046,16 @@
       <c r="AD10" s="3">
         <v>38</v>
       </c>
-      <c r="AE10" s="3"/>
-      <c r="AF10" s="3"/>
-      <c r="AG10" s="3"/>
-      <c r="AH10" s="3"/>
+      <c r="AE10" s="2">
+        <v>38</v>
+      </c>
+      <c r="AF10" s="4">
+        <v>58</v>
+      </c>
+      <c r="AG10" s="4">
+        <v>85</v>
+      </c>
+      <c r="AH10" s="4"/>
       <c r="AI10" s="3"/>
       <c r="AJ10" s="3"/>
       <c r="AK10" s="3"/>
@@ -2002,10 +2151,16 @@
       <c r="AD11" s="3">
         <v>96</v>
       </c>
-      <c r="AE11" s="3"/>
-      <c r="AF11" s="3"/>
-      <c r="AG11" s="3"/>
-      <c r="AH11" s="3"/>
+      <c r="AE11" s="2">
+        <v>97</v>
+      </c>
+      <c r="AF11" s="4">
+        <v>123</v>
+      </c>
+      <c r="AG11" s="4">
+        <v>174</v>
+      </c>
+      <c r="AH11" s="4"/>
       <c r="AI11" s="3"/>
       <c r="AJ11" s="3"/>
       <c r="AK11" s="3"/>
@@ -2101,10 +2256,16 @@
       <c r="AD12" s="3">
         <v>49</v>
       </c>
-      <c r="AE12" s="3"/>
-      <c r="AF12" s="3"/>
-      <c r="AG12" s="3"/>
-      <c r="AH12" s="3"/>
+      <c r="AE12" s="2">
+        <v>49</v>
+      </c>
+      <c r="AF12" s="4">
+        <v>50</v>
+      </c>
+      <c r="AG12" s="4">
+        <v>61</v>
+      </c>
+      <c r="AH12" s="4"/>
       <c r="AI12" s="3"/>
       <c r="AJ12" s="3"/>
       <c r="AK12" s="3"/>
@@ -2200,10 +2361,16 @@
       <c r="AD13" s="3">
         <v>62</v>
       </c>
-      <c r="AE13" s="3"/>
-      <c r="AF13" s="3"/>
-      <c r="AG13" s="3"/>
-      <c r="AH13" s="3"/>
+      <c r="AE13" s="2">
+        <v>62</v>
+      </c>
+      <c r="AF13" s="4">
+        <v>66</v>
+      </c>
+      <c r="AG13" s="4">
+        <v>77</v>
+      </c>
+      <c r="AH13" s="4"/>
       <c r="AI13" s="3"/>
       <c r="AJ13" s="3"/>
       <c r="AK13" s="3"/>
@@ -2299,10 +2466,16 @@
       <c r="AD14" s="3">
         <v>75</v>
       </c>
-      <c r="AE14" s="3"/>
-      <c r="AF14" s="3"/>
-      <c r="AG14" s="3"/>
-      <c r="AH14" s="3"/>
+      <c r="AE14" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF14" s="4">
+        <v>87</v>
+      </c>
+      <c r="AG14" s="4">
+        <v>111</v>
+      </c>
+      <c r="AH14" s="4"/>
       <c r="AI14" s="3"/>
       <c r="AJ14" s="3"/>
       <c r="AK14" s="3"/>
@@ -2398,10 +2571,16 @@
       <c r="AD15" s="3">
         <v>263</v>
       </c>
-      <c r="AE15" s="3"/>
-      <c r="AF15" s="3"/>
-      <c r="AG15" s="3"/>
-      <c r="AH15" s="3"/>
+      <c r="AE15" s="2">
+        <v>263</v>
+      </c>
+      <c r="AF15" s="4">
+        <v>300</v>
+      </c>
+      <c r="AG15" s="4">
+        <v>313</v>
+      </c>
+      <c r="AH15" s="4"/>
       <c r="AI15" s="3"/>
       <c r="AJ15" s="3"/>
       <c r="AK15" s="3"/>
@@ -2497,10 +2676,16 @@
       <c r="AD16" s="3">
         <v>211</v>
       </c>
-      <c r="AE16" s="3"/>
-      <c r="AF16" s="3"/>
-      <c r="AG16" s="3"/>
-      <c r="AH16" s="3"/>
+      <c r="AE16" s="2">
+        <v>211</v>
+      </c>
+      <c r="AF16" s="4">
+        <v>250</v>
+      </c>
+      <c r="AG16" s="4">
+        <v>305</v>
+      </c>
+      <c r="AH16" s="4"/>
       <c r="AI16" s="3"/>
       <c r="AJ16" s="3"/>
       <c r="AK16" s="3"/>
@@ -2596,10 +2781,16 @@
       <c r="AD17" s="3">
         <v>6</v>
       </c>
-      <c r="AE17" s="3"/>
-      <c r="AF17" s="3"/>
-      <c r="AG17" s="3"/>
-      <c r="AH17" s="3"/>
+      <c r="AE17" s="2">
+        <v>6</v>
+      </c>
+      <c r="AF17" s="4">
+        <v>8</v>
+      </c>
+      <c r="AG17" s="4">
+        <v>9</v>
+      </c>
+      <c r="AH17" s="4"/>
       <c r="AI17" s="3"/>
       <c r="AJ17" s="3"/>
       <c r="AK17" s="3"/>
@@ -2695,10 +2886,16 @@
       <c r="AD18" s="3">
         <v>204</v>
       </c>
-      <c r="AE18" s="3"/>
-      <c r="AF18" s="3"/>
-      <c r="AG18" s="3"/>
-      <c r="AH18" s="3"/>
+      <c r="AE18" s="2">
+        <v>204</v>
+      </c>
+      <c r="AF18" s="4">
+        <v>232</v>
+      </c>
+      <c r="AG18" s="4">
+        <v>276</v>
+      </c>
+      <c r="AH18" s="4"/>
       <c r="AI18" s="3"/>
       <c r="AJ18" s="3"/>
       <c r="AK18" s="3"/>
@@ -2794,10 +2991,16 @@
       <c r="AD19" s="3">
         <v>66</v>
       </c>
-      <c r="AE19" s="3"/>
-      <c r="AF19" s="3"/>
-      <c r="AG19" s="3"/>
-      <c r="AH19" s="3"/>
+      <c r="AE19" s="2">
+        <v>70</v>
+      </c>
+      <c r="AF19" s="4">
+        <v>81</v>
+      </c>
+      <c r="AG19" s="4">
+        <v>86</v>
+      </c>
+      <c r="AH19" s="4"/>
       <c r="AI19" s="3"/>
       <c r="AJ19" s="3"/>
       <c r="AK19" s="3"/>
@@ -2893,10 +3096,16 @@
       <c r="AD20" s="3">
         <v>73</v>
       </c>
-      <c r="AE20" s="3"/>
-      <c r="AF20" s="3"/>
-      <c r="AG20" s="3"/>
-      <c r="AH20" s="3"/>
+      <c r="AE20" s="2">
+        <v>79</v>
+      </c>
+      <c r="AF20" s="4">
+        <v>96</v>
+      </c>
+      <c r="AG20" s="4">
+        <v>118</v>
+      </c>
+      <c r="AH20" s="4"/>
       <c r="AI20" s="3"/>
       <c r="AJ20" s="3"/>
       <c r="AK20" s="3"/>
@@ -2992,10 +3201,16 @@
       <c r="AD21" s="3">
         <v>115</v>
       </c>
-      <c r="AE21" s="3"/>
-      <c r="AF21" s="3"/>
-      <c r="AG21" s="3"/>
-      <c r="AH21" s="3"/>
+      <c r="AE21" s="2">
+        <v>117</v>
+      </c>
+      <c r="AF21" s="4">
+        <v>130</v>
+      </c>
+      <c r="AG21" s="4">
+        <v>157</v>
+      </c>
+      <c r="AH21" s="4"/>
       <c r="AI21" s="3"/>
       <c r="AJ21" s="3"/>
       <c r="AK21" s="3"/>
@@ -3091,10 +3306,16 @@
       <c r="AD22" s="3">
         <v>66</v>
       </c>
-      <c r="AE22" s="3"/>
-      <c r="AF22" s="3"/>
-      <c r="AG22" s="3"/>
-      <c r="AH22" s="3"/>
+      <c r="AE22" s="2">
+        <v>67</v>
+      </c>
+      <c r="AF22" s="4">
+        <v>77</v>
+      </c>
+      <c r="AG22" s="4">
+        <v>97</v>
+      </c>
+      <c r="AH22" s="4"/>
       <c r="AI22" s="3"/>
       <c r="AJ22" s="3"/>
       <c r="AK22" s="3"/>
@@ -3190,10 +3411,16 @@
       <c r="AD23" s="3">
         <v>211</v>
       </c>
-      <c r="AE23" s="3"/>
-      <c r="AF23" s="3"/>
-      <c r="AG23" s="3"/>
-      <c r="AH23" s="3"/>
+      <c r="AE23" s="2">
+        <v>211</v>
+      </c>
+      <c r="AF23" s="4">
+        <v>234</v>
+      </c>
+      <c r="AG23" s="4">
+        <v>269</v>
+      </c>
+      <c r="AH23" s="4"/>
       <c r="AI23" s="3"/>
       <c r="AJ23" s="3"/>
       <c r="AK23" s="3"/>
@@ -3289,10 +3516,16 @@
       <c r="AD24" s="3">
         <v>82</v>
       </c>
-      <c r="AE24" s="3"/>
-      <c r="AF24" s="3"/>
-      <c r="AG24" s="3"/>
-      <c r="AH24" s="3"/>
+      <c r="AE24" s="2">
+        <v>82</v>
+      </c>
+      <c r="AF24" s="4">
+        <v>91</v>
+      </c>
+      <c r="AG24" s="4">
+        <v>100</v>
+      </c>
+      <c r="AH24" s="4"/>
       <c r="AI24" s="3"/>
       <c r="AJ24" s="3"/>
       <c r="AK24" s="3"/>
@@ -3388,10 +3621,16 @@
       <c r="AD25" s="3">
         <v>139</v>
       </c>
-      <c r="AE25" s="3"/>
-      <c r="AF25" s="3"/>
-      <c r="AG25" s="3"/>
-      <c r="AH25" s="3"/>
+      <c r="AE25" s="2">
+        <v>139</v>
+      </c>
+      <c r="AF25" s="4">
+        <v>155</v>
+      </c>
+      <c r="AG25" s="4">
+        <v>191</v>
+      </c>
+      <c r="AH25" s="4"/>
       <c r="AI25" s="3"/>
       <c r="AJ25" s="3"/>
       <c r="AK25" s="3"/>
@@ -3487,10 +3726,16 @@
       <c r="AD26" s="3">
         <v>102</v>
       </c>
-      <c r="AE26" s="3"/>
-      <c r="AF26" s="3"/>
-      <c r="AG26" s="3"/>
-      <c r="AH26" s="3"/>
+      <c r="AE26" s="2">
+        <v>102</v>
+      </c>
+      <c r="AF26" s="4">
+        <v>110</v>
+      </c>
+      <c r="AG26" s="4">
+        <v>119</v>
+      </c>
+      <c r="AH26" s="4"/>
       <c r="AI26" s="3"/>
       <c r="AJ26" s="3"/>
       <c r="AK26" s="3"/>
@@ -3586,10 +3831,16 @@
       <c r="AD27" s="3">
         <v>57</v>
       </c>
-      <c r="AE27" s="3"/>
-      <c r="AF27" s="3"/>
-      <c r="AG27" s="3"/>
-      <c r="AH27" s="3"/>
+      <c r="AE27" s="2">
+        <v>57</v>
+      </c>
+      <c r="AF27" s="4">
+        <v>64</v>
+      </c>
+      <c r="AG27" s="4">
+        <v>74</v>
+      </c>
+      <c r="AH27" s="4"/>
       <c r="AI27" s="3"/>
       <c r="AJ27" s="3"/>
       <c r="AK27" s="3"/>
@@ -3685,10 +3936,16 @@
       <c r="AD28" s="3">
         <v>74</v>
       </c>
-      <c r="AE28" s="3"/>
-      <c r="AF28" s="3"/>
-      <c r="AG28" s="3"/>
-      <c r="AH28" s="3"/>
+      <c r="AE28" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF28" s="4">
+        <v>88</v>
+      </c>
+      <c r="AG28" s="4">
+        <v>125</v>
+      </c>
+      <c r="AH28" s="4"/>
       <c r="AI28" s="3"/>
       <c r="AJ28" s="3"/>
       <c r="AK28" s="3"/>
@@ -3784,10 +4041,16 @@
       <c r="AD29" s="3">
         <v>61</v>
       </c>
-      <c r="AE29" s="3"/>
-      <c r="AF29" s="3"/>
-      <c r="AG29" s="3"/>
-      <c r="AH29" s="3"/>
+      <c r="AE29" s="2">
+        <v>62</v>
+      </c>
+      <c r="AF29" s="4">
+        <v>80</v>
+      </c>
+      <c r="AG29" s="4">
+        <v>99</v>
+      </c>
+      <c r="AH29" s="4"/>
       <c r="AI29" s="3"/>
       <c r="AJ29" s="3"/>
       <c r="AK29" s="3"/>
@@ -3883,10 +4146,16 @@
       <c r="AD30" s="3">
         <v>167</v>
       </c>
-      <c r="AE30" s="3"/>
-      <c r="AF30" s="3"/>
-      <c r="AG30" s="3"/>
-      <c r="AH30" s="3"/>
+      <c r="AE30" s="2">
+        <v>195</v>
+      </c>
+      <c r="AF30" s="4">
+        <v>205</v>
+      </c>
+      <c r="AG30" s="4">
+        <v>249</v>
+      </c>
+      <c r="AH30" s="4"/>
       <c r="AI30" s="3"/>
       <c r="AJ30" s="3"/>
       <c r="AK30" s="3"/>
@@ -3982,10 +4251,16 @@
       <c r="AD31" s="3">
         <v>118</v>
       </c>
-      <c r="AE31" s="3"/>
-      <c r="AF31" s="3"/>
-      <c r="AG31" s="3"/>
-      <c r="AH31" s="3"/>
+      <c r="AE31" s="2">
+        <v>136</v>
+      </c>
+      <c r="AF31" s="4">
+        <v>156</v>
+      </c>
+      <c r="AG31" s="4">
+        <v>180</v>
+      </c>
+      <c r="AH31" s="4"/>
       <c r="AI31" s="3"/>
       <c r="AJ31" s="3"/>
       <c r="AK31" s="3"/>
@@ -4081,10 +4356,16 @@
       <c r="AD32" s="3">
         <v>120</v>
       </c>
-      <c r="AE32" s="3"/>
-      <c r="AF32" s="3"/>
-      <c r="AG32" s="3"/>
-      <c r="AH32" s="3"/>
+      <c r="AE32" s="2">
+        <v>125</v>
+      </c>
+      <c r="AF32" s="4">
+        <v>134</v>
+      </c>
+      <c r="AG32" s="4">
+        <v>155</v>
+      </c>
+      <c r="AH32" s="4"/>
       <c r="AI32" s="3"/>
       <c r="AJ32" s="3"/>
       <c r="AK32" s="3"/>
@@ -4180,10 +4461,16 @@
       <c r="AD33" s="3">
         <v>153</v>
       </c>
-      <c r="AE33" s="3"/>
-      <c r="AF33" s="3"/>
-      <c r="AG33" s="3"/>
-      <c r="AH33" s="3"/>
+      <c r="AE33" s="2">
+        <v>196</v>
+      </c>
+      <c r="AF33" s="4">
+        <v>232</v>
+      </c>
+      <c r="AG33" s="4">
+        <v>285</v>
+      </c>
+      <c r="AH33" s="4"/>
       <c r="AI33" s="3"/>
       <c r="AJ33" s="3"/>
       <c r="AK33" s="3"/>
@@ -4279,10 +4566,16 @@
       <c r="AD34" s="3">
         <v>69</v>
       </c>
-      <c r="AE34" s="3"/>
-      <c r="AF34" s="3"/>
-      <c r="AG34" s="3"/>
-      <c r="AH34" s="3"/>
+      <c r="AE34" s="2">
+        <v>79</v>
+      </c>
+      <c r="AF34" s="4">
+        <v>79</v>
+      </c>
+      <c r="AG34" s="4">
+        <v>90</v>
+      </c>
+      <c r="AH34" s="4"/>
       <c r="AI34" s="3"/>
       <c r="AJ34" s="3"/>
       <c r="AK34" s="3"/>
@@ -4378,10 +4671,16 @@
       <c r="AD35" s="3">
         <v>92</v>
       </c>
-      <c r="AE35" s="3"/>
-      <c r="AF35" s="3"/>
-      <c r="AG35" s="3"/>
-      <c r="AH35" s="3"/>
+      <c r="AE35" s="2">
+        <v>107</v>
+      </c>
+      <c r="AF35" s="4">
+        <v>121</v>
+      </c>
+      <c r="AG35" s="4">
+        <v>132</v>
+      </c>
+      <c r="AH35" s="4"/>
       <c r="AI35" s="3"/>
       <c r="AJ35" s="3"/>
       <c r="AK35" s="3"/>
@@ -4477,10 +4776,16 @@
       <c r="AD36" s="3">
         <v>111</v>
       </c>
-      <c r="AE36" s="3"/>
-      <c r="AF36" s="3"/>
-      <c r="AG36" s="3"/>
-      <c r="AH36" s="3"/>
+      <c r="AE36" s="2">
+        <v>128</v>
+      </c>
+      <c r="AF36" s="4">
+        <v>129</v>
+      </c>
+      <c r="AG36" s="4">
+        <v>141</v>
+      </c>
+      <c r="AH36" s="4"/>
       <c r="AI36" s="3"/>
       <c r="AJ36" s="3"/>
       <c r="AK36" s="3"/>
@@ -4576,10 +4881,16 @@
       <c r="AD37" s="3">
         <v>155</v>
       </c>
-      <c r="AE37" s="3"/>
-      <c r="AF37" s="3"/>
-      <c r="AG37" s="3"/>
-      <c r="AH37" s="3"/>
+      <c r="AE37" s="2">
+        <v>167</v>
+      </c>
+      <c r="AF37" s="4">
+        <v>169</v>
+      </c>
+      <c r="AG37" s="4">
+        <v>196</v>
+      </c>
+      <c r="AH37" s="4"/>
       <c r="AI37" s="3"/>
       <c r="AJ37" s="3"/>
       <c r="AK37" s="3"/>
@@ -4675,10 +4986,16 @@
       <c r="AD38" s="3">
         <v>105</v>
       </c>
-      <c r="AE38" s="3"/>
-      <c r="AF38" s="3"/>
-      <c r="AG38" s="3"/>
-      <c r="AH38" s="3"/>
+      <c r="AE38" s="2">
+        <v>116</v>
+      </c>
+      <c r="AF38" s="4">
+        <v>117</v>
+      </c>
+      <c r="AG38" s="4">
+        <v>126</v>
+      </c>
+      <c r="AH38" s="4"/>
       <c r="AI38" s="3"/>
       <c r="AJ38" s="3"/>
       <c r="AK38" s="3"/>
@@ -4774,10 +5091,16 @@
       <c r="AD39" s="3">
         <v>114</v>
       </c>
-      <c r="AE39" s="3"/>
-      <c r="AF39" s="3"/>
-      <c r="AG39" s="3"/>
-      <c r="AH39" s="3"/>
+      <c r="AE39" s="2">
+        <v>129</v>
+      </c>
+      <c r="AF39" s="4">
+        <v>129</v>
+      </c>
+      <c r="AG39" s="4">
+        <v>142</v>
+      </c>
+      <c r="AH39" s="4"/>
       <c r="AI39" s="3"/>
       <c r="AJ39" s="3"/>
       <c r="AK39" s="3"/>
@@ -4873,10 +5196,16 @@
       <c r="AD40" s="3">
         <v>181</v>
       </c>
-      <c r="AE40" s="3"/>
-      <c r="AF40" s="3"/>
-      <c r="AG40" s="3"/>
-      <c r="AH40" s="3"/>
+      <c r="AE40" s="2">
+        <v>186</v>
+      </c>
+      <c r="AF40" s="4">
+        <v>195</v>
+      </c>
+      <c r="AG40" s="4">
+        <v>239</v>
+      </c>
+      <c r="AH40" s="4"/>
       <c r="AI40" s="3"/>
       <c r="AJ40" s="3"/>
       <c r="AK40" s="3"/>
@@ -4972,10 +5301,16 @@
       <c r="AD41" s="3">
         <v>85</v>
       </c>
-      <c r="AE41" s="3"/>
-      <c r="AF41" s="3"/>
-      <c r="AG41" s="3"/>
-      <c r="AH41" s="3"/>
+      <c r="AE41" s="2">
+        <v>86</v>
+      </c>
+      <c r="AF41" s="4">
+        <v>153</v>
+      </c>
+      <c r="AG41" s="4">
+        <v>182</v>
+      </c>
+      <c r="AH41" s="4"/>
       <c r="AI41" s="3"/>
       <c r="AJ41" s="3"/>
       <c r="AK41" s="3"/>
@@ -5071,10 +5406,16 @@
       <c r="AD42" s="3">
         <v>104</v>
       </c>
-      <c r="AE42" s="3"/>
-      <c r="AF42" s="3"/>
-      <c r="AG42" s="3"/>
-      <c r="AH42" s="3"/>
+      <c r="AE42" s="2">
+        <v>115</v>
+      </c>
+      <c r="AF42" s="4">
+        <v>130</v>
+      </c>
+      <c r="AG42" s="4">
+        <v>151</v>
+      </c>
+      <c r="AH42" s="4"/>
       <c r="AI42" s="3"/>
       <c r="AJ42" s="3"/>
       <c r="AK42" s="3"/>
@@ -5170,10 +5511,16 @@
       <c r="AD43" s="3">
         <v>149</v>
       </c>
-      <c r="AE43" s="3"/>
-      <c r="AF43" s="3"/>
-      <c r="AG43" s="3"/>
-      <c r="AH43" s="3"/>
+      <c r="AE43" s="2">
+        <v>181</v>
+      </c>
+      <c r="AF43" s="4">
+        <v>191</v>
+      </c>
+      <c r="AG43" s="4">
+        <v>212</v>
+      </c>
+      <c r="AH43" s="4"/>
       <c r="AI43" s="3"/>
       <c r="AJ43" s="3"/>
       <c r="AK43" s="3"/>
@@ -5269,10 +5616,16 @@
       <c r="AD44" s="3">
         <v>32</v>
       </c>
-      <c r="AE44" s="3"/>
-      <c r="AF44" s="3"/>
-      <c r="AG44" s="3"/>
-      <c r="AH44" s="3"/>
+      <c r="AE44" s="2">
+        <v>36</v>
+      </c>
+      <c r="AF44" s="4">
+        <v>38</v>
+      </c>
+      <c r="AG44" s="4">
+        <v>41</v>
+      </c>
+      <c r="AH44" s="4"/>
       <c r="AI44" s="3"/>
       <c r="AJ44" s="3"/>
       <c r="AK44" s="3"/>
@@ -5368,10 +5721,16 @@
       <c r="AD45" s="3">
         <v>292</v>
       </c>
-      <c r="AE45" s="3"/>
-      <c r="AF45" s="3"/>
-      <c r="AG45" s="3"/>
-      <c r="AH45" s="3"/>
+      <c r="AE45" s="2">
+        <v>303</v>
+      </c>
+      <c r="AF45" s="4">
+        <v>410</v>
+      </c>
+      <c r="AG45" s="4">
+        <v>482</v>
+      </c>
+      <c r="AH45" s="4"/>
       <c r="AI45" s="3"/>
       <c r="AJ45" s="3"/>
       <c r="AK45" s="3"/>
@@ -5467,10 +5826,16 @@
       <c r="AD46" s="3">
         <v>196</v>
       </c>
-      <c r="AE46" s="3"/>
-      <c r="AF46" s="3"/>
-      <c r="AG46" s="3"/>
-      <c r="AH46" s="3"/>
+      <c r="AE46" s="2">
+        <v>209</v>
+      </c>
+      <c r="AF46" s="4">
+        <v>226</v>
+      </c>
+      <c r="AG46" s="4">
+        <v>278</v>
+      </c>
+      <c r="AH46" s="4"/>
       <c r="AI46" s="3"/>
       <c r="AJ46" s="3"/>
       <c r="AK46" s="3"/>
@@ -5566,10 +5931,16 @@
       <c r="AD47" s="3">
         <v>200</v>
       </c>
-      <c r="AE47" s="3"/>
-      <c r="AF47" s="3"/>
-      <c r="AG47" s="3"/>
-      <c r="AH47" s="3"/>
+      <c r="AE47" s="2">
+        <v>227</v>
+      </c>
+      <c r="AF47" s="4">
+        <v>261</v>
+      </c>
+      <c r="AG47" s="4">
+        <v>311</v>
+      </c>
+      <c r="AH47" s="4"/>
       <c r="AI47" s="3"/>
       <c r="AJ47" s="3"/>
       <c r="AK47" s="3"/>
@@ -5665,10 +6036,16 @@
       <c r="AD48" s="3">
         <v>143</v>
       </c>
-      <c r="AE48" s="3"/>
-      <c r="AF48" s="3"/>
-      <c r="AG48" s="3"/>
-      <c r="AH48" s="3"/>
+      <c r="AE48" s="2">
+        <v>157</v>
+      </c>
+      <c r="AF48" s="4">
+        <v>174</v>
+      </c>
+      <c r="AG48" s="4">
+        <v>205</v>
+      </c>
+      <c r="AH48" s="4"/>
       <c r="AI48" s="3"/>
       <c r="AJ48" s="3"/>
       <c r="AK48" s="3"/>
@@ -5764,10 +6141,16 @@
       <c r="AD49" s="3">
         <v>198</v>
       </c>
-      <c r="AE49" s="3"/>
-      <c r="AF49" s="3"/>
-      <c r="AG49" s="3"/>
-      <c r="AH49" s="3"/>
+      <c r="AE49" s="2">
+        <v>198</v>
+      </c>
+      <c r="AF49" s="4">
+        <v>224</v>
+      </c>
+      <c r="AG49" s="4">
+        <v>259</v>
+      </c>
+      <c r="AH49" s="4"/>
       <c r="AI49" s="3"/>
       <c r="AJ49" s="3"/>
       <c r="AK49" s="3"/>
@@ -5863,10 +6246,16 @@
       <c r="AD50" s="3">
         <v>154</v>
       </c>
-      <c r="AE50" s="3"/>
-      <c r="AF50" s="3"/>
-      <c r="AG50" s="3"/>
-      <c r="AH50" s="3"/>
+      <c r="AE50" s="2">
+        <v>156</v>
+      </c>
+      <c r="AF50" s="4">
+        <v>180</v>
+      </c>
+      <c r="AG50" s="4">
+        <v>210</v>
+      </c>
+      <c r="AH50" s="4"/>
       <c r="AI50" s="3"/>
       <c r="AJ50" s="3"/>
       <c r="AK50" s="3"/>
@@ -5962,10 +6351,16 @@
       <c r="AD51" s="3">
         <v>110</v>
       </c>
-      <c r="AE51" s="3"/>
-      <c r="AF51" s="3"/>
-      <c r="AG51" s="3"/>
-      <c r="AH51" s="3"/>
+      <c r="AE51" s="2">
+        <v>120</v>
+      </c>
+      <c r="AF51" s="4">
+        <v>135</v>
+      </c>
+      <c r="AG51" s="4">
+        <v>158</v>
+      </c>
+      <c r="AH51" s="4"/>
       <c r="AI51" s="3"/>
       <c r="AJ51" s="3"/>
       <c r="AK51" s="3"/>
@@ -6061,10 +6456,16 @@
       <c r="AD52" s="3">
         <v>144</v>
       </c>
-      <c r="AE52" s="3"/>
-      <c r="AF52" s="3"/>
-      <c r="AG52" s="3"/>
-      <c r="AH52" s="3"/>
+      <c r="AE52" s="2">
+        <v>164</v>
+      </c>
+      <c r="AF52" s="4">
+        <v>173</v>
+      </c>
+      <c r="AG52" s="4">
+        <v>206</v>
+      </c>
+      <c r="AH52" s="4"/>
       <c r="AI52" s="3"/>
       <c r="AJ52" s="3"/>
       <c r="AK52" s="3"/>
@@ -6160,10 +6561,16 @@
       <c r="AD53" s="3">
         <v>211</v>
       </c>
-      <c r="AE53" s="3"/>
-      <c r="AF53" s="3"/>
-      <c r="AG53" s="3"/>
-      <c r="AH53" s="3"/>
+      <c r="AE53" s="2">
+        <v>211</v>
+      </c>
+      <c r="AF53" s="4">
+        <v>272</v>
+      </c>
+      <c r="AG53" s="4">
+        <v>331</v>
+      </c>
+      <c r="AH53" s="4"/>
       <c r="AI53" s="3"/>
       <c r="AJ53" s="3"/>
       <c r="AK53" s="3"/>
@@ -6259,10 +6666,16 @@
       <c r="AD54" s="3">
         <v>115</v>
       </c>
-      <c r="AE54" s="3"/>
-      <c r="AF54" s="3"/>
-      <c r="AG54" s="3"/>
-      <c r="AH54" s="3"/>
+      <c r="AE54" s="2">
+        <v>116</v>
+      </c>
+      <c r="AF54" s="4">
+        <v>127</v>
+      </c>
+      <c r="AG54" s="4">
+        <v>164</v>
+      </c>
+      <c r="AH54" s="4"/>
       <c r="AI54" s="3"/>
       <c r="AJ54" s="3"/>
       <c r="AK54" s="3"/>
@@ -6358,10 +6771,16 @@
       <c r="AD55" s="3">
         <v>126</v>
       </c>
-      <c r="AE55" s="3"/>
-      <c r="AF55" s="3"/>
-      <c r="AG55" s="3"/>
-      <c r="AH55" s="3"/>
+      <c r="AE55" s="2">
+        <v>126</v>
+      </c>
+      <c r="AF55" s="4">
+        <v>136</v>
+      </c>
+      <c r="AG55" s="4">
+        <v>159</v>
+      </c>
+      <c r="AH55" s="4"/>
       <c r="AI55" s="3"/>
       <c r="AJ55" s="3"/>
       <c r="AK55" s="3"/>
@@ -6457,10 +6876,16 @@
       <c r="AD56" s="3">
         <v>170</v>
       </c>
-      <c r="AE56" s="3"/>
-      <c r="AF56" s="3"/>
-      <c r="AG56" s="3"/>
-      <c r="AH56" s="3"/>
+      <c r="AE56" s="2">
+        <v>185</v>
+      </c>
+      <c r="AF56" s="4">
+        <v>204</v>
+      </c>
+      <c r="AG56" s="4">
+        <v>249</v>
+      </c>
+      <c r="AH56" s="4"/>
       <c r="AI56" s="3"/>
       <c r="AJ56" s="3"/>
       <c r="AK56" s="3"/>
@@ -6556,10 +6981,16 @@
       <c r="AD57" s="3">
         <v>138</v>
       </c>
-      <c r="AE57" s="3"/>
-      <c r="AF57" s="3"/>
-      <c r="AG57" s="3"/>
-      <c r="AH57" s="3"/>
+      <c r="AE57" s="2">
+        <v>151</v>
+      </c>
+      <c r="AF57" s="4">
+        <v>166</v>
+      </c>
+      <c r="AG57" s="4">
+        <v>198</v>
+      </c>
+      <c r="AH57" s="4"/>
       <c r="AI57" s="3"/>
       <c r="AJ57" s="3"/>
       <c r="AK57" s="3"/>
@@ -6655,10 +7086,16 @@
       <c r="AD58" s="3">
         <v>323</v>
       </c>
-      <c r="AE58" s="3"/>
-      <c r="AF58" s="3"/>
-      <c r="AG58" s="3"/>
-      <c r="AH58" s="3"/>
+      <c r="AE58" s="2">
+        <v>361</v>
+      </c>
+      <c r="AF58" s="4">
+        <v>395</v>
+      </c>
+      <c r="AG58" s="4">
+        <v>512</v>
+      </c>
+      <c r="AH58" s="4"/>
       <c r="AI58" s="3"/>
       <c r="AJ58" s="3"/>
       <c r="AK58" s="3"/>
@@ -6754,10 +7191,16 @@
       <c r="AD59" s="3">
         <v>216</v>
       </c>
-      <c r="AE59" s="3"/>
-      <c r="AF59" s="3"/>
-      <c r="AG59" s="3"/>
-      <c r="AH59" s="3"/>
+      <c r="AE59" s="2">
+        <v>232</v>
+      </c>
+      <c r="AF59" s="4">
+        <v>248</v>
+      </c>
+      <c r="AG59" s="4">
+        <v>284</v>
+      </c>
+      <c r="AH59" s="4"/>
       <c r="AI59" s="3"/>
       <c r="AJ59" s="3"/>
       <c r="AK59" s="3"/>
@@ -6853,10 +7296,16 @@
       <c r="AD60" s="3">
         <v>167</v>
       </c>
-      <c r="AE60" s="3"/>
-      <c r="AF60" s="3"/>
-      <c r="AG60" s="3"/>
-      <c r="AH60" s="3"/>
+      <c r="AE60" s="2">
+        <v>186</v>
+      </c>
+      <c r="AF60" s="4">
+        <v>195</v>
+      </c>
+      <c r="AG60" s="4">
+        <v>222</v>
+      </c>
+      <c r="AH60" s="4"/>
       <c r="AI60" s="3"/>
       <c r="AJ60" s="3"/>
       <c r="AK60" s="3"/>
@@ -6952,10 +7401,16 @@
       <c r="AD61" s="3">
         <v>242</v>
       </c>
-      <c r="AE61" s="3"/>
-      <c r="AF61" s="3"/>
-      <c r="AG61" s="3"/>
-      <c r="AH61" s="3"/>
+      <c r="AE61" s="2">
+        <v>259</v>
+      </c>
+      <c r="AF61" s="4">
+        <v>273</v>
+      </c>
+      <c r="AG61" s="4">
+        <v>310</v>
+      </c>
+      <c r="AH61" s="4"/>
       <c r="AI61" s="3"/>
       <c r="AJ61" s="3"/>
       <c r="AK61" s="3"/>
@@ -7051,10 +7506,16 @@
       <c r="AD62" s="3">
         <v>246</v>
       </c>
-      <c r="AE62" s="3"/>
-      <c r="AF62" s="3"/>
-      <c r="AG62" s="3"/>
-      <c r="AH62" s="3"/>
+      <c r="AE62" s="2">
+        <v>270</v>
+      </c>
+      <c r="AF62" s="4">
+        <v>298</v>
+      </c>
+      <c r="AG62" s="4">
+        <v>368</v>
+      </c>
+      <c r="AH62" s="4"/>
       <c r="AI62" s="3"/>
       <c r="AJ62" s="3"/>
       <c r="AK62" s="3"/>
@@ -7150,10 +7611,16 @@
       <c r="AD63" s="3">
         <v>162</v>
       </c>
-      <c r="AE63" s="3"/>
-      <c r="AF63" s="3"/>
-      <c r="AG63" s="3"/>
-      <c r="AH63" s="3"/>
+      <c r="AE63" s="2">
+        <v>182</v>
+      </c>
+      <c r="AF63" s="4">
+        <v>191</v>
+      </c>
+      <c r="AG63" s="4">
+        <v>227</v>
+      </c>
+      <c r="AH63" s="4"/>
       <c r="AI63" s="3"/>
       <c r="AJ63" s="3"/>
       <c r="AK63" s="3"/>
@@ -7249,10 +7716,16 @@
       <c r="AD64" s="3">
         <v>222</v>
       </c>
-      <c r="AE64" s="3"/>
-      <c r="AF64" s="3"/>
-      <c r="AG64" s="3"/>
-      <c r="AH64" s="3"/>
+      <c r="AE64" s="2">
+        <v>240</v>
+      </c>
+      <c r="AF64" s="4">
+        <v>257</v>
+      </c>
+      <c r="AG64" s="4">
+        <v>297</v>
+      </c>
+      <c r="AH64" s="4"/>
       <c r="AI64" s="3"/>
       <c r="AJ64" s="3"/>
       <c r="AK64" s="3"/>
@@ -7348,10 +7821,16 @@
       <c r="AD65" s="3">
         <v>185</v>
       </c>
-      <c r="AE65" s="3"/>
-      <c r="AF65" s="3"/>
-      <c r="AG65" s="3"/>
-      <c r="AH65" s="3"/>
+      <c r="AE65" s="2">
+        <v>197</v>
+      </c>
+      <c r="AF65" s="4">
+        <v>209</v>
+      </c>
+      <c r="AG65" s="4">
+        <v>253</v>
+      </c>
+      <c r="AH65" s="4"/>
       <c r="AI65" s="3"/>
       <c r="AJ65" s="3"/>
       <c r="AK65" s="3"/>
@@ -7447,10 +7926,16 @@
       <c r="AD66" s="3">
         <v>167</v>
       </c>
-      <c r="AE66" s="3"/>
-      <c r="AF66" s="3"/>
-      <c r="AG66" s="3"/>
-      <c r="AH66" s="3"/>
+      <c r="AE66" s="2">
+        <v>169</v>
+      </c>
+      <c r="AF66" s="4">
+        <v>198</v>
+      </c>
+      <c r="AG66" s="4">
+        <v>245</v>
+      </c>
+      <c r="AH66" s="4"/>
       <c r="AI66" s="3"/>
       <c r="AJ66" s="3"/>
       <c r="AK66" s="3"/>
@@ -7546,10 +8031,16 @@
       <c r="AD67" s="3">
         <v>510</v>
       </c>
-      <c r="AE67" s="3"/>
-      <c r="AF67" s="3"/>
-      <c r="AG67" s="3"/>
-      <c r="AH67" s="3"/>
+      <c r="AE67" s="2">
+        <v>552</v>
+      </c>
+      <c r="AF67" s="4">
+        <v>587</v>
+      </c>
+      <c r="AG67" s="4">
+        <v>702</v>
+      </c>
+      <c r="AH67" s="4"/>
       <c r="AI67" s="3"/>
       <c r="AJ67" s="3"/>
       <c r="AK67" s="3"/>
@@ -7645,10 +8136,16 @@
       <c r="AD68" s="3">
         <v>236</v>
       </c>
-      <c r="AE68" s="3"/>
-      <c r="AF68" s="3"/>
-      <c r="AG68" s="3"/>
-      <c r="AH68" s="3"/>
+      <c r="AE68" s="2">
+        <v>239</v>
+      </c>
+      <c r="AF68" s="4">
+        <v>269</v>
+      </c>
+      <c r="AG68" s="4">
+        <v>329</v>
+      </c>
+      <c r="AH68" s="4"/>
       <c r="AI68" s="3"/>
       <c r="AJ68" s="3"/>
       <c r="AK68" s="3"/>
@@ -7744,10 +8241,16 @@
       <c r="AD69" s="3">
         <v>264</v>
       </c>
-      <c r="AE69" s="3"/>
-      <c r="AF69" s="3"/>
-      <c r="AG69" s="3"/>
-      <c r="AH69" s="3"/>
+      <c r="AE69" s="2">
+        <v>289</v>
+      </c>
+      <c r="AF69" s="4">
+        <v>306</v>
+      </c>
+      <c r="AG69" s="4">
+        <v>387</v>
+      </c>
+      <c r="AH69" s="4"/>
       <c r="AI69" s="3"/>
       <c r="AJ69" s="3"/>
       <c r="AK69" s="3"/>
@@ -7843,10 +8346,16 @@
       <c r="AD70" s="3">
         <v>220</v>
       </c>
-      <c r="AE70" s="3"/>
-      <c r="AF70" s="3"/>
-      <c r="AG70" s="3"/>
-      <c r="AH70" s="3"/>
+      <c r="AE70" s="2">
+        <v>262</v>
+      </c>
+      <c r="AF70" s="4">
+        <v>288</v>
+      </c>
+      <c r="AG70" s="4">
+        <v>385</v>
+      </c>
+      <c r="AH70" s="4"/>
       <c r="AI70" s="3"/>
       <c r="AJ70" s="3"/>
       <c r="AK70" s="3"/>
@@ -7942,10 +8451,16 @@
       <c r="AD71" s="3">
         <v>216</v>
       </c>
-      <c r="AE71" s="3"/>
-      <c r="AF71" s="3"/>
-      <c r="AG71" s="3"/>
-      <c r="AH71" s="3"/>
+      <c r="AE71" s="2">
+        <v>216</v>
+      </c>
+      <c r="AF71" s="4">
+        <v>238</v>
+      </c>
+      <c r="AG71" s="4">
+        <v>267</v>
+      </c>
+      <c r="AH71" s="4"/>
       <c r="AI71" s="3"/>
       <c r="AJ71" s="3"/>
       <c r="AK71" s="3"/>
@@ -8041,10 +8556,16 @@
       <c r="AD72" s="3">
         <v>144</v>
       </c>
-      <c r="AE72" s="3"/>
-      <c r="AF72" s="3"/>
-      <c r="AG72" s="3"/>
-      <c r="AH72" s="3"/>
+      <c r="AE72" s="2">
+        <v>144</v>
+      </c>
+      <c r="AF72" s="4">
+        <v>168</v>
+      </c>
+      <c r="AG72" s="4">
+        <v>183</v>
+      </c>
+      <c r="AH72" s="4"/>
       <c r="AI72" s="3"/>
       <c r="AJ72" s="3"/>
       <c r="AK72" s="3"/>
@@ -8140,10 +8661,16 @@
       <c r="AD73" s="3">
         <v>221</v>
       </c>
-      <c r="AE73" s="3"/>
-      <c r="AF73" s="3"/>
-      <c r="AG73" s="3"/>
-      <c r="AH73" s="3"/>
+      <c r="AE73" s="2">
+        <v>223</v>
+      </c>
+      <c r="AF73" s="4">
+        <v>240</v>
+      </c>
+      <c r="AG73" s="4">
+        <v>279</v>
+      </c>
+      <c r="AH73" s="4"/>
       <c r="AI73" s="3"/>
       <c r="AJ73" s="3"/>
       <c r="AK73" s="3"/>
@@ -8239,10 +8766,16 @@
       <c r="AD74" s="3">
         <v>882</v>
       </c>
-      <c r="AE74" s="3"/>
-      <c r="AF74" s="3"/>
-      <c r="AG74" s="3"/>
-      <c r="AH74" s="3"/>
+      <c r="AE74" s="2">
+        <v>883</v>
+      </c>
+      <c r="AF74" s="4">
+        <v>940</v>
+      </c>
+      <c r="AG74" s="4">
+        <v>1095</v>
+      </c>
+      <c r="AH74" s="4"/>
       <c r="AI74" s="3"/>
       <c r="AJ74" s="3"/>
       <c r="AK74" s="3"/>
@@ -8338,10 +8871,16 @@
       <c r="AD75" s="3">
         <v>359</v>
       </c>
-      <c r="AE75" s="3"/>
-      <c r="AF75" s="3"/>
-      <c r="AG75" s="3"/>
-      <c r="AH75" s="3"/>
+      <c r="AE75" s="2">
+        <v>367</v>
+      </c>
+      <c r="AF75" s="4">
+        <v>432</v>
+      </c>
+      <c r="AG75" s="4">
+        <v>493</v>
+      </c>
+      <c r="AH75" s="4"/>
       <c r="AI75" s="3"/>
       <c r="AJ75" s="3"/>
       <c r="AK75" s="3"/>
@@ -8437,10 +8976,16 @@
       <c r="AD76" s="3">
         <v>180</v>
       </c>
-      <c r="AE76" s="3"/>
-      <c r="AF76" s="3"/>
-      <c r="AG76" s="3"/>
-      <c r="AH76" s="3"/>
+      <c r="AE76" s="2">
+        <v>183</v>
+      </c>
+      <c r="AF76" s="4">
+        <v>242</v>
+      </c>
+      <c r="AG76" s="4">
+        <v>276</v>
+      </c>
+      <c r="AH76" s="4"/>
       <c r="AI76" s="3"/>
       <c r="AJ76" s="3"/>
       <c r="AK76" s="3"/>
@@ -8536,10 +9081,16 @@
       <c r="AD77" s="3">
         <v>98</v>
       </c>
-      <c r="AE77" s="3"/>
-      <c r="AF77" s="3"/>
-      <c r="AG77" s="3"/>
-      <c r="AH77" s="3"/>
+      <c r="AE77" s="2">
+        <v>101</v>
+      </c>
+      <c r="AF77" s="4">
+        <v>118</v>
+      </c>
+      <c r="AG77" s="4">
+        <v>123</v>
+      </c>
+      <c r="AH77" s="4"/>
       <c r="AI77" s="3"/>
       <c r="AJ77" s="3"/>
       <c r="AK77" s="3"/>
@@ -8635,10 +9186,16 @@
       <c r="AD78" s="3">
         <v>278</v>
       </c>
-      <c r="AE78" s="3"/>
-      <c r="AF78" s="3"/>
-      <c r="AG78" s="3"/>
-      <c r="AH78" s="3"/>
+      <c r="AE78" s="2">
+        <v>285</v>
+      </c>
+      <c r="AF78" s="4">
+        <v>343</v>
+      </c>
+      <c r="AG78" s="4">
+        <v>354</v>
+      </c>
+      <c r="AH78" s="4"/>
       <c r="AI78" s="3"/>
       <c r="AJ78" s="3"/>
       <c r="AK78" s="3"/>
@@ -8734,10 +9291,16 @@
       <c r="AD79" s="3">
         <v>1287</v>
       </c>
-      <c r="AE79" s="3"/>
-      <c r="AF79" s="3"/>
-      <c r="AG79" s="3"/>
-      <c r="AH79" s="3"/>
+      <c r="AE79" s="2">
+        <v>1372</v>
+      </c>
+      <c r="AF79" s="4">
+        <v>1462</v>
+      </c>
+      <c r="AG79" s="4">
+        <v>1604</v>
+      </c>
+      <c r="AH79" s="4"/>
       <c r="AI79" s="3"/>
       <c r="AJ79" s="3"/>
       <c r="AK79" s="3"/>
@@ -8833,10 +9396,16 @@
       <c r="AD80" s="3">
         <v>263</v>
       </c>
-      <c r="AE80" s="3"/>
-      <c r="AF80" s="3"/>
-      <c r="AG80" s="3"/>
-      <c r="AH80" s="3"/>
+      <c r="AE80" s="2">
+        <v>277</v>
+      </c>
+      <c r="AF80" s="4">
+        <v>295</v>
+      </c>
+      <c r="AG80" s="4">
+        <v>335</v>
+      </c>
+      <c r="AH80" s="4"/>
       <c r="AI80" s="3"/>
       <c r="AJ80" s="3"/>
       <c r="AK80" s="3"/>
@@ -8932,10 +9501,16 @@
       <c r="AD81" s="3">
         <v>296</v>
       </c>
-      <c r="AE81" s="3"/>
-      <c r="AF81" s="3"/>
-      <c r="AG81" s="3"/>
-      <c r="AH81" s="3"/>
+      <c r="AE81" s="2">
+        <v>309</v>
+      </c>
+      <c r="AF81" s="4">
+        <v>341</v>
+      </c>
+      <c r="AG81" s="4">
+        <v>379</v>
+      </c>
+      <c r="AH81" s="4"/>
       <c r="AI81" s="3"/>
       <c r="AJ81" s="3"/>
       <c r="AK81" s="3"/>
@@ -9031,10 +9606,16 @@
       <c r="AD82" s="3">
         <v>353</v>
       </c>
-      <c r="AE82" s="3"/>
-      <c r="AF82" s="3"/>
-      <c r="AG82" s="3"/>
-      <c r="AH82" s="3"/>
+      <c r="AE82" s="2">
+        <v>363</v>
+      </c>
+      <c r="AF82" s="4">
+        <v>399</v>
+      </c>
+      <c r="AG82" s="4">
+        <v>448</v>
+      </c>
+      <c r="AH82" s="4"/>
       <c r="AI82" s="3"/>
       <c r="AJ82" s="3"/>
       <c r="AK82" s="3"/>
@@ -9130,10 +9711,16 @@
       <c r="AD83" s="3">
         <v>215</v>
       </c>
-      <c r="AE83" s="3"/>
-      <c r="AF83" s="3"/>
-      <c r="AG83" s="3"/>
-      <c r="AH83" s="3"/>
+      <c r="AE83" s="2">
+        <v>241</v>
+      </c>
+      <c r="AF83" s="4">
+        <v>259</v>
+      </c>
+      <c r="AG83" s="4">
+        <v>284</v>
+      </c>
+      <c r="AH83" s="4"/>
       <c r="AI83" s="3"/>
       <c r="AJ83" s="3"/>
       <c r="AK83" s="3"/>
@@ -9229,10 +9816,16 @@
       <c r="AD84" s="3">
         <v>359</v>
       </c>
-      <c r="AE84" s="3"/>
-      <c r="AF84" s="3"/>
-      <c r="AG84" s="3"/>
-      <c r="AH84" s="3"/>
+      <c r="AE84" s="2">
+        <v>386</v>
+      </c>
+      <c r="AF84" s="4">
+        <v>421</v>
+      </c>
+      <c r="AG84" s="4">
+        <v>461</v>
+      </c>
+      <c r="AH84" s="4"/>
       <c r="AI84" s="3"/>
       <c r="AJ84" s="3"/>
       <c r="AK84" s="3"/>
@@ -9328,10 +9921,16 @@
       <c r="AD85" s="3">
         <v>304</v>
       </c>
-      <c r="AE85" s="3"/>
-      <c r="AF85" s="3"/>
-      <c r="AG85" s="3"/>
-      <c r="AH85" s="3"/>
+      <c r="AE85" s="2">
+        <v>335</v>
+      </c>
+      <c r="AF85" s="4">
+        <v>354</v>
+      </c>
+      <c r="AG85" s="4">
+        <v>388</v>
+      </c>
+      <c r="AH85" s="4"/>
       <c r="AI85" s="3"/>
       <c r="AJ85" s="3"/>
       <c r="AK85" s="3"/>
@@ -9427,10 +10026,16 @@
       <c r="AD86" s="3">
         <v>204</v>
       </c>
-      <c r="AE86" s="3"/>
-      <c r="AF86" s="3"/>
-      <c r="AG86" s="3"/>
-      <c r="AH86" s="3"/>
+      <c r="AE86" s="2">
+        <v>222</v>
+      </c>
+      <c r="AF86" s="4">
+        <v>258</v>
+      </c>
+      <c r="AG86" s="4">
+        <v>331</v>
+      </c>
+      <c r="AH86" s="4"/>
       <c r="AI86" s="3"/>
       <c r="AJ86" s="3"/>
       <c r="AK86" s="3"/>
@@ -9526,10 +10131,16 @@
       <c r="AD87" s="3">
         <v>94</v>
       </c>
-      <c r="AE87" s="3"/>
-      <c r="AF87" s="3"/>
-      <c r="AG87" s="3"/>
-      <c r="AH87" s="3"/>
+      <c r="AE87" s="2">
+        <v>94</v>
+      </c>
+      <c r="AF87" s="4">
+        <v>110</v>
+      </c>
+      <c r="AG87" s="4">
+        <v>122</v>
+      </c>
+      <c r="AH87" s="4"/>
       <c r="AI87" s="3"/>
       <c r="AJ87" s="3"/>
       <c r="AK87" s="3"/>
@@ -9625,10 +10236,16 @@
       <c r="AD88" s="3">
         <v>198</v>
       </c>
-      <c r="AE88" s="3"/>
-      <c r="AF88" s="3"/>
-      <c r="AG88" s="3"/>
-      <c r="AH88" s="3"/>
+      <c r="AE88" s="2">
+        <v>203</v>
+      </c>
+      <c r="AF88" s="4">
+        <v>235</v>
+      </c>
+      <c r="AG88" s="4">
+        <v>278</v>
+      </c>
+      <c r="AH88" s="4"/>
       <c r="AI88" s="3"/>
       <c r="AJ88" s="3"/>
       <c r="AK88" s="3"/>
@@ -9724,10 +10341,16 @@
       <c r="AD89" s="3">
         <v>325</v>
       </c>
-      <c r="AE89" s="3"/>
-      <c r="AF89" s="3"/>
-      <c r="AG89" s="3"/>
-      <c r="AH89" s="3"/>
+      <c r="AE89" s="2">
+        <v>340</v>
+      </c>
+      <c r="AF89" s="4">
+        <v>389</v>
+      </c>
+      <c r="AG89" s="4">
+        <v>504</v>
+      </c>
+      <c r="AH89" s="4"/>
       <c r="AI89" s="3"/>
       <c r="AJ89" s="3"/>
       <c r="AK89" s="3"/>
@@ -9823,10 +10446,16 @@
       <c r="AD90" s="3">
         <v>162</v>
       </c>
-      <c r="AE90" s="3"/>
-      <c r="AF90" s="3"/>
-      <c r="AG90" s="3"/>
-      <c r="AH90" s="3"/>
+      <c r="AE90" s="2">
+        <v>177</v>
+      </c>
+      <c r="AF90" s="4">
+        <v>200</v>
+      </c>
+      <c r="AG90" s="4">
+        <v>245</v>
+      </c>
+      <c r="AH90" s="4"/>
       <c r="AI90" s="3"/>
       <c r="AJ90" s="3"/>
       <c r="AK90" s="3"/>
@@ -9922,10 +10551,16 @@
       <c r="AD91" s="3">
         <v>180</v>
       </c>
-      <c r="AE91" s="3"/>
-      <c r="AF91" s="3"/>
-      <c r="AG91" s="3"/>
-      <c r="AH91" s="3"/>
+      <c r="AE91" s="2">
+        <v>188</v>
+      </c>
+      <c r="AF91" s="4">
+        <v>230</v>
+      </c>
+      <c r="AG91" s="4">
+        <v>247</v>
+      </c>
+      <c r="AH91" s="4"/>
       <c r="AI91" s="3"/>
       <c r="AJ91" s="3"/>
       <c r="AK91" s="3"/>
@@ -10021,10 +10656,16 @@
       <c r="AD92" s="3">
         <v>211</v>
       </c>
-      <c r="AE92" s="3"/>
-      <c r="AF92" s="3"/>
-      <c r="AG92" s="3"/>
-      <c r="AH92" s="3"/>
+      <c r="AE92" s="2">
+        <v>222</v>
+      </c>
+      <c r="AF92" s="4">
+        <v>249</v>
+      </c>
+      <c r="AG92" s="4">
+        <v>279</v>
+      </c>
+      <c r="AH92" s="4"/>
       <c r="AI92" s="3"/>
       <c r="AJ92" s="3"/>
       <c r="AK92" s="3"/>
@@ -10120,10 +10761,16 @@
       <c r="AD93" s="3">
         <v>666</v>
       </c>
-      <c r="AE93" s="3"/>
-      <c r="AF93" s="3"/>
-      <c r="AG93" s="3"/>
-      <c r="AH93" s="3"/>
+      <c r="AE93" s="2">
+        <v>717</v>
+      </c>
+      <c r="AF93" s="4">
+        <v>752</v>
+      </c>
+      <c r="AG93" s="4">
+        <v>837</v>
+      </c>
+      <c r="AH93" s="4"/>
       <c r="AI93" s="3"/>
       <c r="AJ93" s="3"/>
       <c r="AK93" s="3"/>
@@ -10219,10 +10866,16 @@
       <c r="AD94" s="3">
         <v>250</v>
       </c>
-      <c r="AE94" s="3"/>
-      <c r="AF94" s="3"/>
-      <c r="AG94" s="3"/>
-      <c r="AH94" s="3"/>
+      <c r="AE94" s="2">
+        <v>274</v>
+      </c>
+      <c r="AF94" s="4">
+        <v>303</v>
+      </c>
+      <c r="AG94" s="4">
+        <v>374</v>
+      </c>
+      <c r="AH94" s="4"/>
       <c r="AI94" s="3"/>
       <c r="AJ94" s="3"/>
       <c r="AK94" s="3"/>
@@ -10318,10 +10971,16 @@
       <c r="AD95" s="3">
         <v>759</v>
       </c>
-      <c r="AE95" s="3"/>
-      <c r="AF95" s="3"/>
-      <c r="AG95" s="3"/>
-      <c r="AH95" s="3"/>
+      <c r="AE95" s="2">
+        <v>819</v>
+      </c>
+      <c r="AF95" s="4">
+        <v>853</v>
+      </c>
+      <c r="AG95" s="4">
+        <v>912</v>
+      </c>
+      <c r="AH95" s="4"/>
       <c r="AI95" s="3"/>
       <c r="AJ95" s="3"/>
       <c r="AK95" s="3"/>
@@ -10417,10 +11076,16 @@
       <c r="AD96" s="3">
         <v>521</v>
       </c>
-      <c r="AE96" s="3"/>
-      <c r="AF96" s="3"/>
-      <c r="AG96" s="3"/>
-      <c r="AH96" s="3"/>
+      <c r="AE96" s="2">
+        <v>547</v>
+      </c>
+      <c r="AF96" s="4">
+        <v>583</v>
+      </c>
+      <c r="AG96" s="4">
+        <v>658</v>
+      </c>
+      <c r="AH96" s="4"/>
       <c r="AI96" s="3"/>
       <c r="AJ96" s="3"/>
       <c r="AK96" s="3"/>
@@ -10516,10 +11181,16 @@
       <c r="AD97" s="3">
         <v>298</v>
       </c>
-      <c r="AE97" s="3"/>
-      <c r="AF97" s="3"/>
-      <c r="AG97" s="3"/>
-      <c r="AH97" s="3"/>
+      <c r="AE97" s="2">
+        <v>321</v>
+      </c>
+      <c r="AF97" s="4">
+        <v>343</v>
+      </c>
+      <c r="AG97" s="4">
+        <v>373</v>
+      </c>
+      <c r="AH97" s="4"/>
       <c r="AI97" s="3"/>
       <c r="AJ97" s="3"/>
       <c r="AK97" s="3"/>
@@ -10615,10 +11286,16 @@
       <c r="AD98" s="3">
         <v>620</v>
       </c>
-      <c r="AE98" s="3"/>
-      <c r="AF98" s="3"/>
-      <c r="AG98" s="3"/>
-      <c r="AH98" s="3"/>
+      <c r="AE98" s="2">
+        <v>689</v>
+      </c>
+      <c r="AF98" s="4">
+        <v>763</v>
+      </c>
+      <c r="AG98" s="4">
+        <v>853</v>
+      </c>
+      <c r="AH98" s="4"/>
       <c r="AI98" s="3"/>
       <c r="AJ98" s="3"/>
       <c r="AK98" s="3"/>
@@ -10714,10 +11391,16 @@
       <c r="AD99" s="3">
         <v>503</v>
       </c>
-      <c r="AE99" s="3"/>
-      <c r="AF99" s="3"/>
-      <c r="AG99" s="3"/>
-      <c r="AH99" s="3"/>
+      <c r="AE99" s="2">
+        <v>533</v>
+      </c>
+      <c r="AF99" s="4">
+        <v>553</v>
+      </c>
+      <c r="AG99" s="4">
+        <v>624</v>
+      </c>
+      <c r="AH99" s="4"/>
       <c r="AI99" s="3"/>
       <c r="AJ99" s="3"/>
       <c r="AK99" s="3"/>
@@ -10813,10 +11496,16 @@
       <c r="AD100" s="3">
         <v>350</v>
       </c>
-      <c r="AE100" s="3"/>
-      <c r="AF100" s="3"/>
-      <c r="AG100" s="3"/>
-      <c r="AH100" s="3"/>
+      <c r="AE100" s="2">
+        <v>370</v>
+      </c>
+      <c r="AF100" s="4">
+        <v>392</v>
+      </c>
+      <c r="AG100" s="4">
+        <v>434</v>
+      </c>
+      <c r="AH100" s="4"/>
       <c r="AI100" s="3"/>
       <c r="AJ100" s="3"/>
       <c r="AK100" s="3"/>
@@ -10912,10 +11601,16 @@
       <c r="AD101" s="3">
         <v>322</v>
       </c>
-      <c r="AE101" s="3"/>
-      <c r="AF101" s="3"/>
-      <c r="AG101" s="3"/>
-      <c r="AH101" s="3"/>
+      <c r="AE101" s="2">
+        <v>337</v>
+      </c>
+      <c r="AF101" s="4">
+        <v>378</v>
+      </c>
+      <c r="AG101" s="4">
+        <v>432</v>
+      </c>
+      <c r="AH101" s="4"/>
       <c r="AI101" s="3"/>
       <c r="AJ101" s="3"/>
       <c r="AK101" s="3"/>
@@ -11011,10 +11706,16 @@
       <c r="AD102" s="3">
         <v>362</v>
       </c>
-      <c r="AE102" s="3"/>
-      <c r="AF102" s="3"/>
-      <c r="AG102" s="3"/>
-      <c r="AH102" s="3"/>
+      <c r="AE102" s="2">
+        <v>365</v>
+      </c>
+      <c r="AF102" s="4">
+        <v>412</v>
+      </c>
+      <c r="AG102" s="4">
+        <v>470</v>
+      </c>
+      <c r="AH102" s="4"/>
       <c r="AI102" s="3"/>
       <c r="AJ102" s="3"/>
       <c r="AK102" s="3"/>
@@ -11110,10 +11811,16 @@
       <c r="AD103" s="3">
         <v>266</v>
       </c>
-      <c r="AE103" s="3"/>
-      <c r="AF103" s="3"/>
-      <c r="AG103" s="3"/>
-      <c r="AH103" s="3"/>
+      <c r="AE103" s="2">
+        <v>286</v>
+      </c>
+      <c r="AF103" s="4">
+        <v>295</v>
+      </c>
+      <c r="AG103" s="4">
+        <v>332</v>
+      </c>
+      <c r="AH103" s="4"/>
       <c r="AI103" s="3"/>
       <c r="AJ103" s="3"/>
       <c r="AK103" s="3"/>
@@ -11209,10 +11916,16 @@
       <c r="AD104" s="3">
         <v>285</v>
       </c>
-      <c r="AE104" s="3"/>
-      <c r="AF104" s="3"/>
-      <c r="AG104" s="3"/>
-      <c r="AH104" s="3"/>
+      <c r="AE104" s="2">
+        <v>308</v>
+      </c>
+      <c r="AF104" s="4">
+        <v>324</v>
+      </c>
+      <c r="AG104" s="4">
+        <v>349</v>
+      </c>
+      <c r="AH104" s="4"/>
       <c r="AI104" s="3"/>
       <c r="AJ104" s="3"/>
       <c r="AK104" s="3"/>
@@ -11308,10 +12021,16 @@
       <c r="AD105" s="3">
         <v>469</v>
       </c>
-      <c r="AE105" s="3"/>
-      <c r="AF105" s="3"/>
-      <c r="AG105" s="3"/>
-      <c r="AH105" s="3"/>
+      <c r="AE105" s="2">
+        <v>500</v>
+      </c>
+      <c r="AF105" s="4">
+        <v>530</v>
+      </c>
+      <c r="AG105" s="4">
+        <v>574</v>
+      </c>
+      <c r="AH105" s="4"/>
       <c r="AI105" s="3"/>
       <c r="AJ105" s="3"/>
       <c r="AK105" s="3"/>
@@ -11407,10 +12126,16 @@
       <c r="AD106" s="3">
         <v>248</v>
       </c>
-      <c r="AE106" s="3"/>
-      <c r="AF106" s="3"/>
-      <c r="AG106" s="3"/>
-      <c r="AH106" s="3"/>
+      <c r="AE106" s="2">
+        <v>273</v>
+      </c>
+      <c r="AF106" s="4">
+        <v>299</v>
+      </c>
+      <c r="AG106" s="4">
+        <v>372</v>
+      </c>
+      <c r="AH106" s="4"/>
       <c r="AI106" s="3"/>
       <c r="AJ106" s="3"/>
       <c r="AK106" s="3"/>
@@ -11506,10 +12231,16 @@
       <c r="AD107" s="3">
         <v>348</v>
       </c>
-      <c r="AE107" s="3"/>
-      <c r="AF107" s="3"/>
-      <c r="AG107" s="3"/>
-      <c r="AH107" s="3"/>
+      <c r="AE107" s="2">
+        <v>366</v>
+      </c>
+      <c r="AF107" s="4">
+        <v>389</v>
+      </c>
+      <c r="AG107" s="4">
+        <v>434</v>
+      </c>
+      <c r="AH107" s="4"/>
       <c r="AI107" s="3"/>
       <c r="AJ107" s="3"/>
       <c r="AK107" s="3"/>
@@ -11605,10 +12336,16 @@
       <c r="AD108" s="3">
         <v>338</v>
       </c>
-      <c r="AE108" s="3"/>
-      <c r="AF108" s="3"/>
-      <c r="AG108" s="3"/>
-      <c r="AH108" s="3"/>
+      <c r="AE108" s="2">
+        <v>361</v>
+      </c>
+      <c r="AF108" s="4">
+        <v>380</v>
+      </c>
+      <c r="AG108" s="4">
+        <v>416</v>
+      </c>
+      <c r="AH108" s="4"/>
       <c r="AI108" s="3"/>
       <c r="AJ108" s="3"/>
       <c r="AK108" s="3"/>
@@ -11704,10 +12441,16 @@
       <c r="AD109" s="3">
         <v>257</v>
       </c>
-      <c r="AE109" s="3"/>
-      <c r="AF109" s="3"/>
-      <c r="AG109" s="3"/>
-      <c r="AH109" s="3"/>
+      <c r="AE109" s="2">
+        <v>268</v>
+      </c>
+      <c r="AF109" s="4">
+        <v>276</v>
+      </c>
+      <c r="AG109" s="4">
+        <v>290</v>
+      </c>
+      <c r="AH109" s="4"/>
       <c r="AI109" s="3"/>
       <c r="AJ109" s="3"/>
       <c r="AK109" s="3"/>
@@ -11803,10 +12546,16 @@
       <c r="AD110" s="3">
         <v>272</v>
       </c>
-      <c r="AE110" s="3"/>
-      <c r="AF110" s="3"/>
-      <c r="AG110" s="3"/>
-      <c r="AH110" s="3"/>
+      <c r="AE110" s="2">
+        <v>278</v>
+      </c>
+      <c r="AF110" s="4">
+        <v>286</v>
+      </c>
+      <c r="AG110" s="4">
+        <v>314</v>
+      </c>
+      <c r="AH110" s="4"/>
       <c r="AI110" s="3"/>
       <c r="AJ110" s="3"/>
       <c r="AK110" s="3"/>
@@ -11902,10 +12651,16 @@
       <c r="AD111" s="3">
         <v>169</v>
       </c>
-      <c r="AE111" s="3"/>
-      <c r="AF111" s="3"/>
-      <c r="AG111" s="3"/>
-      <c r="AH111" s="3"/>
+      <c r="AE111" s="2">
+        <v>199</v>
+      </c>
+      <c r="AF111" s="4">
+        <v>212</v>
+      </c>
+      <c r="AG111" s="4">
+        <v>244</v>
+      </c>
+      <c r="AH111" s="4"/>
       <c r="AI111" s="3"/>
       <c r="AJ111" s="3"/>
       <c r="AK111" s="3"/>
@@ -12001,10 +12756,16 @@
       <c r="AD112" s="3">
         <v>671</v>
       </c>
-      <c r="AE112" s="3"/>
-      <c r="AF112" s="3"/>
-      <c r="AG112" s="3"/>
-      <c r="AH112" s="3"/>
+      <c r="AE112" s="2">
+        <v>698</v>
+      </c>
+      <c r="AF112" s="4">
+        <v>731</v>
+      </c>
+      <c r="AG112" s="4">
+        <v>794</v>
+      </c>
+      <c r="AH112" s="4"/>
       <c r="AI112" s="3"/>
       <c r="AJ112" s="3"/>
       <c r="AK112" s="3"/>
@@ -12100,10 +12861,16 @@
       <c r="AD113" s="3">
         <v>490</v>
       </c>
-      <c r="AE113" s="3"/>
-      <c r="AF113" s="3"/>
-      <c r="AG113" s="3"/>
-      <c r="AH113" s="3"/>
+      <c r="AE113" s="2">
+        <v>516</v>
+      </c>
+      <c r="AF113" s="4">
+        <v>554</v>
+      </c>
+      <c r="AG113" s="4">
+        <v>644</v>
+      </c>
+      <c r="AH113" s="4"/>
       <c r="AI113" s="3"/>
       <c r="AJ113" s="3"/>
       <c r="AK113" s="3"/>
@@ -12199,10 +12966,16 @@
       <c r="AD114" s="3">
         <v>316</v>
       </c>
-      <c r="AE114" s="3"/>
-      <c r="AF114" s="3"/>
-      <c r="AG114" s="3"/>
-      <c r="AH114" s="3"/>
+      <c r="AE114" s="2">
+        <v>358</v>
+      </c>
+      <c r="AF114" s="4">
+        <v>386</v>
+      </c>
+      <c r="AG114" s="4">
+        <v>440</v>
+      </c>
+      <c r="AH114" s="4"/>
       <c r="AI114" s="3"/>
       <c r="AJ114" s="3"/>
       <c r="AK114" s="3"/>
@@ -12298,10 +13071,16 @@
       <c r="AD115" s="3">
         <v>530</v>
       </c>
-      <c r="AE115" s="3"/>
-      <c r="AF115" s="3"/>
-      <c r="AG115" s="3"/>
-      <c r="AH115" s="3"/>
+      <c r="AE115" s="2">
+        <v>535</v>
+      </c>
+      <c r="AF115" s="4">
+        <v>608</v>
+      </c>
+      <c r="AG115" s="4">
+        <v>684</v>
+      </c>
+      <c r="AH115" s="4"/>
       <c r="AI115" s="3"/>
       <c r="AJ115" s="3"/>
       <c r="AK115" s="3"/>
@@ -12397,10 +13176,16 @@
       <c r="AD116" s="3">
         <v>311</v>
       </c>
-      <c r="AE116" s="3"/>
-      <c r="AF116" s="3"/>
-      <c r="AG116" s="3"/>
-      <c r="AH116" s="3"/>
+      <c r="AE116" s="2">
+        <v>319</v>
+      </c>
+      <c r="AF116" s="4">
+        <v>366</v>
+      </c>
+      <c r="AG116" s="4">
+        <v>436</v>
+      </c>
+      <c r="AH116" s="4"/>
       <c r="AI116" s="3"/>
       <c r="AJ116" s="3"/>
       <c r="AK116" s="3"/>
@@ -12496,10 +13281,16 @@
       <c r="AD117" s="3">
         <v>200</v>
       </c>
-      <c r="AE117" s="3"/>
-      <c r="AF117" s="3"/>
-      <c r="AG117" s="3"/>
-      <c r="AH117" s="3"/>
+      <c r="AE117" s="2">
+        <v>213</v>
+      </c>
+      <c r="AF117" s="4">
+        <v>223</v>
+      </c>
+      <c r="AG117" s="4">
+        <v>247</v>
+      </c>
+      <c r="AH117" s="4"/>
       <c r="AI117" s="3"/>
       <c r="AJ117" s="3"/>
       <c r="AK117" s="3"/>
@@ -12595,10 +13386,16 @@
       <c r="AD118" s="3">
         <v>685</v>
       </c>
-      <c r="AE118" s="3"/>
-      <c r="AF118" s="3"/>
-      <c r="AG118" s="3"/>
-      <c r="AH118" s="3"/>
+      <c r="AE118" s="2">
+        <v>710</v>
+      </c>
+      <c r="AF118" s="4">
+        <v>755</v>
+      </c>
+      <c r="AG118" s="4">
+        <v>826</v>
+      </c>
+      <c r="AH118" s="4"/>
       <c r="AI118" s="3"/>
       <c r="AJ118" s="3"/>
       <c r="AK118" s="3"/>
@@ -12694,10 +13491,16 @@
       <c r="AD119" s="3">
         <v>262</v>
       </c>
-      <c r="AE119" s="3"/>
-      <c r="AF119" s="3"/>
-      <c r="AG119" s="3"/>
-      <c r="AH119" s="3"/>
+      <c r="AE119" s="2">
+        <v>287</v>
+      </c>
+      <c r="AF119" s="4">
+        <v>299</v>
+      </c>
+      <c r="AG119" s="4">
+        <v>349</v>
+      </c>
+      <c r="AH119" s="4"/>
       <c r="AI119" s="3"/>
       <c r="AJ119" s="3"/>
       <c r="AK119" s="3"/>
@@ -12793,10 +13596,16 @@
       <c r="AD120" s="3">
         <v>359</v>
       </c>
-      <c r="AE120" s="3"/>
-      <c r="AF120" s="3"/>
-      <c r="AG120" s="3"/>
-      <c r="AH120" s="3"/>
+      <c r="AE120" s="2">
+        <v>361</v>
+      </c>
+      <c r="AF120" s="4">
+        <v>406</v>
+      </c>
+      <c r="AG120" s="4">
+        <v>448</v>
+      </c>
+      <c r="AH120" s="4"/>
       <c r="AI120" s="3"/>
       <c r="AJ120" s="3"/>
       <c r="AK120" s="3"/>
@@ -12892,10 +13701,16 @@
       <c r="AD121" s="3">
         <v>389</v>
       </c>
-      <c r="AE121" s="3"/>
-      <c r="AF121" s="3"/>
-      <c r="AG121" s="3"/>
-      <c r="AH121" s="3"/>
+      <c r="AE121" s="2">
+        <v>393</v>
+      </c>
+      <c r="AF121" s="4">
+        <v>443</v>
+      </c>
+      <c r="AG121" s="4">
+        <v>478</v>
+      </c>
+      <c r="AH121" s="4"/>
       <c r="AI121" s="3"/>
       <c r="AJ121" s="3"/>
       <c r="AK121" s="3"/>
@@ -12991,10 +13806,16 @@
       <c r="AD122" s="3">
         <v>526</v>
       </c>
-      <c r="AE122" s="3"/>
-      <c r="AF122" s="3"/>
-      <c r="AG122" s="3"/>
-      <c r="AH122" s="3"/>
+      <c r="AE122" s="2">
+        <v>557</v>
+      </c>
+      <c r="AF122" s="4">
+        <v>592</v>
+      </c>
+      <c r="AG122" s="4">
+        <v>650</v>
+      </c>
+      <c r="AH122" s="4"/>
       <c r="AI122" s="3"/>
       <c r="AJ122" s="3"/>
       <c r="AK122" s="3"/>
@@ -13090,10 +13911,16 @@
       <c r="AD123" s="3">
         <v>383</v>
       </c>
-      <c r="AE123" s="3"/>
-      <c r="AF123" s="3"/>
-      <c r="AG123" s="3"/>
-      <c r="AH123" s="3"/>
+      <c r="AE123" s="2">
+        <v>398</v>
+      </c>
+      <c r="AF123" s="4">
+        <v>420</v>
+      </c>
+      <c r="AG123" s="4">
+        <v>444</v>
+      </c>
+      <c r="AH123" s="4"/>
       <c r="AI123" s="3"/>
       <c r="AJ123" s="3"/>
       <c r="AK123" s="3"/>
@@ -13189,10 +14016,16 @@
       <c r="AD124" s="3">
         <v>300</v>
       </c>
-      <c r="AE124" s="3"/>
-      <c r="AF124" s="3"/>
-      <c r="AG124" s="3"/>
-      <c r="AH124" s="3"/>
+      <c r="AE124" s="2">
+        <v>329</v>
+      </c>
+      <c r="AF124" s="4">
+        <v>342</v>
+      </c>
+      <c r="AG124" s="4">
+        <v>391</v>
+      </c>
+      <c r="AH124" s="4"/>
       <c r="AI124" s="3"/>
       <c r="AJ124" s="3"/>
       <c r="AK124" s="3"/>
@@ -13288,10 +14121,16 @@
       <c r="AD125" s="3">
         <v>222</v>
       </c>
-      <c r="AE125" s="3"/>
-      <c r="AF125" s="3"/>
-      <c r="AG125" s="3"/>
-      <c r="AH125" s="3"/>
+      <c r="AE125" s="2">
+        <v>237</v>
+      </c>
+      <c r="AF125" s="4">
+        <v>278</v>
+      </c>
+      <c r="AG125" s="4">
+        <v>320</v>
+      </c>
+      <c r="AH125" s="4"/>
       <c r="AI125" s="3"/>
       <c r="AJ125" s="3"/>
       <c r="AK125" s="3"/>
@@ -13387,10 +14226,16 @@
       <c r="AD126" s="3">
         <v>753</v>
       </c>
-      <c r="AE126" s="3"/>
-      <c r="AF126" s="3"/>
-      <c r="AG126" s="3"/>
-      <c r="AH126" s="3"/>
+      <c r="AE126" s="2">
+        <v>804</v>
+      </c>
+      <c r="AF126" s="4">
+        <v>864</v>
+      </c>
+      <c r="AG126" s="4">
+        <v>1023</v>
+      </c>
+      <c r="AH126" s="4"/>
       <c r="AI126" s="3"/>
       <c r="AJ126" s="3"/>
       <c r="AK126" s="3"/>
@@ -13486,10 +14331,16 @@
       <c r="AD127" s="3">
         <v>494</v>
       </c>
-      <c r="AE127" s="3"/>
-      <c r="AF127" s="3"/>
-      <c r="AG127" s="3"/>
-      <c r="AH127" s="3"/>
+      <c r="AE127" s="2">
+        <v>501</v>
+      </c>
+      <c r="AF127" s="4">
+        <v>555</v>
+      </c>
+      <c r="AG127" s="4">
+        <v>603</v>
+      </c>
+      <c r="AH127" s="4"/>
       <c r="AI127" s="3"/>
       <c r="AJ127" s="3"/>
       <c r="AK127" s="3"/>
@@ -13585,10 +14436,16 @@
       <c r="AD128" s="3">
         <v>229</v>
       </c>
-      <c r="AE128" s="3"/>
-      <c r="AF128" s="3"/>
-      <c r="AG128" s="3"/>
-      <c r="AH128" s="3"/>
+      <c r="AE128" s="2">
+        <v>236</v>
+      </c>
+      <c r="AF128" s="4">
+        <v>250</v>
+      </c>
+      <c r="AG128" s="4">
+        <v>312</v>
+      </c>
+      <c r="AH128" s="4"/>
       <c r="AI128" s="3"/>
       <c r="AJ128" s="3"/>
       <c r="AK128" s="3"/>
@@ -13684,10 +14541,16 @@
       <c r="AD129" s="3">
         <v>161</v>
       </c>
-      <c r="AE129" s="3"/>
-      <c r="AF129" s="3"/>
-      <c r="AG129" s="3"/>
-      <c r="AH129" s="3"/>
+      <c r="AE129" s="2">
+        <v>181</v>
+      </c>
+      <c r="AF129" s="4">
+        <v>229</v>
+      </c>
+      <c r="AG129" s="4">
+        <v>301</v>
+      </c>
+      <c r="AH129" s="4"/>
       <c r="AI129" s="3"/>
       <c r="AJ129" s="3"/>
       <c r="AK129" s="3"/>
@@ -13783,10 +14646,16 @@
       <c r="AD130" s="3">
         <v>858</v>
       </c>
-      <c r="AE130" s="3"/>
-      <c r="AF130" s="3"/>
-      <c r="AG130" s="3"/>
-      <c r="AH130" s="3"/>
+      <c r="AE130" s="2">
+        <v>938</v>
+      </c>
+      <c r="AF130" s="4">
+        <v>1081</v>
+      </c>
+      <c r="AG130" s="4">
+        <v>1232</v>
+      </c>
+      <c r="AH130" s="4"/>
       <c r="AI130" s="3"/>
       <c r="AJ130" s="3"/>
       <c r="AK130" s="3"/>
@@ -13882,10 +14751,16 @@
       <c r="AD131" s="3">
         <v>306</v>
       </c>
-      <c r="AE131" s="3"/>
-      <c r="AF131" s="3"/>
-      <c r="AG131" s="3"/>
-      <c r="AH131" s="3"/>
+      <c r="AE131" s="2">
+        <v>364</v>
+      </c>
+      <c r="AF131" s="4">
+        <v>402</v>
+      </c>
+      <c r="AG131" s="4">
+        <v>496</v>
+      </c>
+      <c r="AH131" s="4"/>
       <c r="AI131" s="3"/>
       <c r="AJ131" s="3"/>
       <c r="AK131" s="3"/>
@@ -13981,10 +14856,16 @@
       <c r="AD132" s="3">
         <v>921</v>
       </c>
-      <c r="AE132" s="3"/>
-      <c r="AF132" s="3"/>
-      <c r="AG132" s="3"/>
-      <c r="AH132" s="3"/>
+      <c r="AE132" s="2">
+        <v>989</v>
+      </c>
+      <c r="AF132" s="4">
+        <v>1241</v>
+      </c>
+      <c r="AG132" s="4">
+        <v>1416</v>
+      </c>
+      <c r="AH132" s="4"/>
       <c r="AI132" s="3"/>
       <c r="AJ132" s="3"/>
       <c r="AK132" s="3"/>
@@ -14080,10 +14961,16 @@
       <c r="AD133" s="3">
         <v>870</v>
       </c>
-      <c r="AE133" s="3"/>
-      <c r="AF133" s="3"/>
-      <c r="AG133" s="3"/>
-      <c r="AH133" s="3"/>
+      <c r="AE133" s="2">
+        <v>933</v>
+      </c>
+      <c r="AF133" s="4">
+        <v>1032</v>
+      </c>
+      <c r="AG133" s="4">
+        <v>1179</v>
+      </c>
+      <c r="AH133" s="4"/>
       <c r="AI133" s="3"/>
       <c r="AJ133" s="3"/>
       <c r="AK133" s="3"/>
@@ -14179,10 +15066,16 @@
       <c r="AD134" s="3">
         <v>791</v>
       </c>
-      <c r="AE134" s="3"/>
-      <c r="AF134" s="3"/>
-      <c r="AG134" s="3"/>
-      <c r="AH134" s="3"/>
+      <c r="AE134" s="2">
+        <v>923</v>
+      </c>
+      <c r="AF134" s="4">
+        <v>1033</v>
+      </c>
+      <c r="AG134" s="4">
+        <v>1252</v>
+      </c>
+      <c r="AH134" s="4"/>
       <c r="AI134" s="3"/>
       <c r="AJ134" s="3"/>
       <c r="AK134" s="3"/>
@@ -14278,10 +15171,16 @@
       <c r="AD135" s="3">
         <v>838</v>
       </c>
-      <c r="AE135" s="3"/>
-      <c r="AF135" s="3"/>
-      <c r="AG135" s="3"/>
-      <c r="AH135" s="3"/>
+      <c r="AE135" s="2">
+        <v>923</v>
+      </c>
+      <c r="AF135" s="4">
+        <v>1026</v>
+      </c>
+      <c r="AG135" s="4">
+        <v>1226</v>
+      </c>
+      <c r="AH135" s="4"/>
       <c r="AI135" s="3"/>
       <c r="AJ135" s="3"/>
       <c r="AK135" s="3"/>
@@ -14377,10 +15276,16 @@
       <c r="AD136" s="3">
         <v>338</v>
       </c>
-      <c r="AE136" s="3"/>
-      <c r="AF136" s="3"/>
-      <c r="AG136" s="3"/>
-      <c r="AH136" s="3"/>
+      <c r="AE136" s="2">
+        <v>339</v>
+      </c>
+      <c r="AF136" s="4">
+        <v>386</v>
+      </c>
+      <c r="AG136" s="4">
+        <v>449</v>
+      </c>
+      <c r="AH136" s="4"/>
       <c r="AI136" s="3"/>
       <c r="AJ136" s="3"/>
       <c r="AK136" s="3"/>
@@ -14476,10 +15381,16 @@
       <c r="AD137" s="3">
         <v>275</v>
       </c>
-      <c r="AE137" s="3"/>
-      <c r="AF137" s="3"/>
-      <c r="AG137" s="3"/>
-      <c r="AH137" s="3"/>
+      <c r="AE137" s="2">
+        <v>277</v>
+      </c>
+      <c r="AF137" s="4">
+        <v>319</v>
+      </c>
+      <c r="AG137" s="4">
+        <v>392</v>
+      </c>
+      <c r="AH137" s="4"/>
       <c r="AI137" s="3"/>
       <c r="AJ137" s="3"/>
       <c r="AK137" s="3"/>
@@ -14575,10 +15486,16 @@
       <c r="AD138" s="3">
         <v>301</v>
       </c>
-      <c r="AE138" s="3"/>
-      <c r="AF138" s="3"/>
-      <c r="AG138" s="3"/>
-      <c r="AH138" s="3"/>
+      <c r="AE138" s="2">
+        <v>341</v>
+      </c>
+      <c r="AF138" s="4">
+        <v>386</v>
+      </c>
+      <c r="AG138" s="4">
+        <v>486</v>
+      </c>
+      <c r="AH138" s="4"/>
       <c r="AI138" s="3"/>
       <c r="AJ138" s="3"/>
       <c r="AK138" s="3"/>
@@ -14674,10 +15591,16 @@
       <c r="AD139" s="3">
         <v>428</v>
       </c>
-      <c r="AE139" s="3"/>
-      <c r="AF139" s="3"/>
-      <c r="AG139" s="3"/>
-      <c r="AH139" s="3"/>
+      <c r="AE139" s="2">
+        <v>473</v>
+      </c>
+      <c r="AF139" s="4">
+        <v>536</v>
+      </c>
+      <c r="AG139" s="4">
+        <v>626</v>
+      </c>
+      <c r="AH139" s="4"/>
       <c r="AI139" s="3"/>
       <c r="AJ139" s="3"/>
       <c r="AK139" s="3"/>
@@ -14773,10 +15696,16 @@
       <c r="AD140" s="3">
         <v>269</v>
       </c>
-      <c r="AE140" s="3"/>
-      <c r="AF140" s="3"/>
-      <c r="AG140" s="3"/>
-      <c r="AH140" s="3"/>
+      <c r="AE140" s="2">
+        <v>285</v>
+      </c>
+      <c r="AF140" s="4">
+        <v>328</v>
+      </c>
+      <c r="AG140" s="4">
+        <v>390</v>
+      </c>
+      <c r="AH140" s="4"/>
       <c r="AI140" s="3"/>
       <c r="AJ140" s="3"/>
       <c r="AK140" s="3"/>
@@ -14872,10 +15801,16 @@
       <c r="AD141" s="3">
         <v>425</v>
       </c>
-      <c r="AE141" s="3"/>
-      <c r="AF141" s="3"/>
-      <c r="AG141" s="3"/>
-      <c r="AH141" s="3"/>
+      <c r="AE141" s="2">
+        <v>469</v>
+      </c>
+      <c r="AF141" s="4">
+        <v>509</v>
+      </c>
+      <c r="AG141" s="4">
+        <v>566</v>
+      </c>
+      <c r="AH141" s="4"/>
       <c r="AI141" s="3"/>
       <c r="AJ141" s="3"/>
       <c r="AK141" s="3"/>
@@ -14971,10 +15906,16 @@
       <c r="AD142" s="3">
         <v>450</v>
       </c>
-      <c r="AE142" s="3"/>
-      <c r="AF142" s="3"/>
-      <c r="AG142" s="3"/>
-      <c r="AH142" s="3"/>
+      <c r="AE142" s="2">
+        <v>501</v>
+      </c>
+      <c r="AF142" s="4">
+        <v>533</v>
+      </c>
+      <c r="AG142" s="4">
+        <v>653</v>
+      </c>
+      <c r="AH142" s="4"/>
       <c r="AI142" s="3"/>
       <c r="AJ142" s="3"/>
       <c r="AK142" s="3"/>
@@ -15070,10 +16011,16 @@
       <c r="AD143" s="3">
         <v>114</v>
       </c>
-      <c r="AE143" s="3"/>
-      <c r="AF143" s="3"/>
-      <c r="AG143" s="3"/>
-      <c r="AH143" s="3"/>
+      <c r="AE143" s="2">
+        <v>114</v>
+      </c>
+      <c r="AF143" s="4">
+        <v>135</v>
+      </c>
+      <c r="AG143" s="4">
+        <v>168</v>
+      </c>
+      <c r="AH143" s="4"/>
       <c r="AI143" s="3"/>
       <c r="AJ143" s="3"/>
       <c r="AK143" s="3"/>
@@ -15169,10 +16116,16 @@
       <c r="AD144" s="3">
         <v>570</v>
       </c>
-      <c r="AE144" s="3"/>
-      <c r="AF144" s="3"/>
-      <c r="AG144" s="3"/>
-      <c r="AH144" s="3"/>
+      <c r="AE144" s="2">
+        <v>597</v>
+      </c>
+      <c r="AF144" s="4">
+        <v>673</v>
+      </c>
+      <c r="AG144" s="4">
+        <v>760</v>
+      </c>
+      <c r="AH144" s="4"/>
       <c r="AI144" s="3"/>
       <c r="AJ144" s="3"/>
       <c r="AK144" s="3"/>
@@ -15268,10 +16221,16 @@
       <c r="AD145" s="3">
         <v>243</v>
       </c>
-      <c r="AE145" s="3"/>
-      <c r="AF145" s="3"/>
-      <c r="AG145" s="3"/>
-      <c r="AH145" s="3"/>
+      <c r="AE145" s="2">
+        <v>263</v>
+      </c>
+      <c r="AF145" s="4">
+        <v>302</v>
+      </c>
+      <c r="AG145" s="4">
+        <v>360</v>
+      </c>
+      <c r="AH145" s="4"/>
       <c r="AI145" s="3"/>
       <c r="AJ145" s="3"/>
       <c r="AK145" s="3"/>
@@ -15367,10 +16326,16 @@
       <c r="AD146" s="3">
         <v>887</v>
       </c>
-      <c r="AE146" s="3"/>
-      <c r="AF146" s="3"/>
-      <c r="AG146" s="3"/>
-      <c r="AH146" s="3"/>
+      <c r="AE146" s="2">
+        <v>1017</v>
+      </c>
+      <c r="AF146" s="4">
+        <v>1059</v>
+      </c>
+      <c r="AG146" s="4">
+        <v>1238</v>
+      </c>
+      <c r="AH146" s="4"/>
       <c r="AI146" s="3"/>
       <c r="AJ146" s="3"/>
       <c r="AK146" s="3"/>
@@ -15466,10 +16431,16 @@
       <c r="AD147" s="3">
         <v>361</v>
       </c>
-      <c r="AE147" s="3"/>
-      <c r="AF147" s="3"/>
-      <c r="AG147" s="3"/>
-      <c r="AH147" s="3"/>
+      <c r="AE147" s="2">
+        <v>400</v>
+      </c>
+      <c r="AF147" s="4">
+        <v>439</v>
+      </c>
+      <c r="AG147" s="4">
+        <v>513</v>
+      </c>
+      <c r="AH147" s="4"/>
       <c r="AI147" s="3"/>
       <c r="AJ147" s="3"/>
       <c r="AK147" s="3"/>
@@ -15565,10 +16536,16 @@
       <c r="AD148" s="3">
         <v>224</v>
       </c>
-      <c r="AE148" s="3"/>
-      <c r="AF148" s="3"/>
-      <c r="AG148" s="3"/>
-      <c r="AH148" s="3"/>
+      <c r="AE148" s="2">
+        <v>266</v>
+      </c>
+      <c r="AF148" s="4">
+        <v>320</v>
+      </c>
+      <c r="AG148" s="4">
+        <v>363</v>
+      </c>
+      <c r="AH148" s="4"/>
       <c r="AI148" s="3"/>
       <c r="AJ148" s="3"/>
       <c r="AK148" s="3"/>
@@ -15664,10 +16641,16 @@
       <c r="AD149" s="3">
         <v>394</v>
       </c>
-      <c r="AE149" s="3"/>
-      <c r="AF149" s="3"/>
-      <c r="AG149" s="3"/>
-      <c r="AH149" s="3"/>
+      <c r="AE149" s="2">
+        <v>419</v>
+      </c>
+      <c r="AF149" s="4">
+        <v>439</v>
+      </c>
+      <c r="AG149" s="4">
+        <v>508</v>
+      </c>
+      <c r="AH149" s="4"/>
       <c r="AI149" s="3"/>
       <c r="AJ149" s="3"/>
       <c r="AK149" s="3"/>

</xml_diff>